<commit_message>
transaction verifier flow completed
</commit_message>
<xml_diff>
--- a/src/main/resources/Bulk_ConventionalTransactions_File.xlsx
+++ b/src/main/resources/Bulk_ConventionalTransactions_File.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\BDD_Framework\30 March\10MayNew\upp-test-automation\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24401" uniqueCount="656">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24593" uniqueCount="841">
   <si>
     <t>transactionName</t>
   </si>
@@ -1951,9 +1951,6 @@
     <t>123</t>
   </si>
   <si>
-    <t>Manisha transaction1</t>
-  </si>
-  <si>
     <t>Payment</t>
   </si>
   <si>
@@ -1972,22 +1969,580 @@
     <t>ADD2</t>
   </si>
   <si>
-    <t>Manisha transactio21</t>
-  </si>
-  <si>
-    <t>PASS</t>
-  </si>
-  <si>
-    <t>tran2710905855</t>
-  </si>
-  <si>
-    <t>transaction12710905855</t>
-  </si>
-  <si>
-    <t>6543234</t>
-  </si>
-  <si>
-    <t>76567894</t>
+    <t>tran31562851993</t>
+  </si>
+  <si>
+    <t>transaction131563285199</t>
+  </si>
+  <si>
+    <t>tran2220410189</t>
+  </si>
+  <si>
+    <t>transaction12220410189</t>
+  </si>
+  <si>
+    <t>5926839309</t>
+  </si>
+  <si>
+    <t>1917075353</t>
+  </si>
+  <si>
+    <t>tran3168975030</t>
+  </si>
+  <si>
+    <t>transaction13168975030</t>
+  </si>
+  <si>
+    <t>9720385224</t>
+  </si>
+  <si>
+    <t>2869605032</t>
+  </si>
+  <si>
+    <t>tran2675526863</t>
+  </si>
+  <si>
+    <t>transaction12675526863</t>
+  </si>
+  <si>
+    <t>1360284043</t>
+  </si>
+  <si>
+    <t>6692107930</t>
+  </si>
+  <si>
+    <t>tran4563878273</t>
+  </si>
+  <si>
+    <t>transaction14563878273</t>
+  </si>
+  <si>
+    <t>2174591355</t>
+  </si>
+  <si>
+    <t>8397647418</t>
+  </si>
+  <si>
+    <t>tran2536298242</t>
+  </si>
+  <si>
+    <t>transaction12536298242</t>
+  </si>
+  <si>
+    <t>7201670404</t>
+  </si>
+  <si>
+    <t>3606527842</t>
+  </si>
+  <si>
+    <t>tran6018555551</t>
+  </si>
+  <si>
+    <t>transaction16018555551</t>
+  </si>
+  <si>
+    <t>4080447587</t>
+  </si>
+  <si>
+    <t>4554549065</t>
+  </si>
+  <si>
+    <t>tran4810984332</t>
+  </si>
+  <si>
+    <t>transaction14810984332</t>
+  </si>
+  <si>
+    <t>4353486664</t>
+  </si>
+  <si>
+    <t>9631293769</t>
+  </si>
+  <si>
+    <t>tran1033549629</t>
+  </si>
+  <si>
+    <t>transaction11033549629</t>
+  </si>
+  <si>
+    <t>7875127720</t>
+  </si>
+  <si>
+    <t>3203268155</t>
+  </si>
+  <si>
+    <t>tran4386579392</t>
+  </si>
+  <si>
+    <t>transaction14386579392</t>
+  </si>
+  <si>
+    <t>2188908755</t>
+  </si>
+  <si>
+    <t>1749649300</t>
+  </si>
+  <si>
+    <t>tran4547006125</t>
+  </si>
+  <si>
+    <t>transaction14547006125</t>
+  </si>
+  <si>
+    <t>2189716657</t>
+  </si>
+  <si>
+    <t>6689142101</t>
+  </si>
+  <si>
+    <t>tran1242020376</t>
+  </si>
+  <si>
+    <t>transaction11242020376</t>
+  </si>
+  <si>
+    <t>9648715418</t>
+  </si>
+  <si>
+    <t>3309382468</t>
+  </si>
+  <si>
+    <t>tran9878986976</t>
+  </si>
+  <si>
+    <t>transaction19878986976</t>
+  </si>
+  <si>
+    <t>6804857608</t>
+  </si>
+  <si>
+    <t>6054139799</t>
+  </si>
+  <si>
+    <t>tran7084720137</t>
+  </si>
+  <si>
+    <t>transaction17084720137</t>
+  </si>
+  <si>
+    <t>7595892522</t>
+  </si>
+  <si>
+    <t>6646597229</t>
+  </si>
+  <si>
+    <t>tran2798396314</t>
+  </si>
+  <si>
+    <t>transaction12798396314</t>
+  </si>
+  <si>
+    <t>5927640401</t>
+  </si>
+  <si>
+    <t>1574612081</t>
+  </si>
+  <si>
+    <t>tran7420727064</t>
+  </si>
+  <si>
+    <t>transaction17420727064</t>
+  </si>
+  <si>
+    <t>4854969548</t>
+  </si>
+  <si>
+    <t>7337787878</t>
+  </si>
+  <si>
+    <t>tran7454406510</t>
+  </si>
+  <si>
+    <t>transaction17454406510</t>
+  </si>
+  <si>
+    <t>7415668699</t>
+  </si>
+  <si>
+    <t>7185795517</t>
+  </si>
+  <si>
+    <t>tran8736375407</t>
+  </si>
+  <si>
+    <t>transaction18736375407</t>
+  </si>
+  <si>
+    <t>7332437496</t>
+  </si>
+  <si>
+    <t>8739602199</t>
+  </si>
+  <si>
+    <t>tran7853762411</t>
+  </si>
+  <si>
+    <t>transaction17853762411</t>
+  </si>
+  <si>
+    <t>7622005242</t>
+  </si>
+  <si>
+    <t>6947382697</t>
+  </si>
+  <si>
+    <t>tran1897754676</t>
+  </si>
+  <si>
+    <t>transaction11897754676</t>
+  </si>
+  <si>
+    <t>7237888936</t>
+  </si>
+  <si>
+    <t>8607114659</t>
+  </si>
+  <si>
+    <t>tran4895374326</t>
+  </si>
+  <si>
+    <t>transaction14895374326</t>
+  </si>
+  <si>
+    <t>3006292919</t>
+  </si>
+  <si>
+    <t>2499900981</t>
+  </si>
+  <si>
+    <t>tran5462140886</t>
+  </si>
+  <si>
+    <t>transaction15462140886</t>
+  </si>
+  <si>
+    <t>2539719545</t>
+  </si>
+  <si>
+    <t>9883845829</t>
+  </si>
+  <si>
+    <t>tran2862118519</t>
+  </si>
+  <si>
+    <t>transaction12862118519</t>
+  </si>
+  <si>
+    <t>5355501345</t>
+  </si>
+  <si>
+    <t>4151484857</t>
+  </si>
+  <si>
+    <t>tran5827868989</t>
+  </si>
+  <si>
+    <t>transaction15827868989</t>
+  </si>
+  <si>
+    <t>7345037513</t>
+  </si>
+  <si>
+    <t>7643266198</t>
+  </si>
+  <si>
+    <t>tran1942908760</t>
+  </si>
+  <si>
+    <t>transaction11942908760</t>
+  </si>
+  <si>
+    <t>1122062616</t>
+  </si>
+  <si>
+    <t>6050676410</t>
+  </si>
+  <si>
+    <t>tran7785455375</t>
+  </si>
+  <si>
+    <t>transaction17785455375</t>
+  </si>
+  <si>
+    <t>1160598615</t>
+  </si>
+  <si>
+    <t>5601738662</t>
+  </si>
+  <si>
+    <t>tran7329995884</t>
+  </si>
+  <si>
+    <t>transaction17329995884</t>
+  </si>
+  <si>
+    <t>1357910765</t>
+  </si>
+  <si>
+    <t>2709621822</t>
+  </si>
+  <si>
+    <t>tran7778548431</t>
+  </si>
+  <si>
+    <t>transaction17778548431</t>
+  </si>
+  <si>
+    <t>8439142179</t>
+  </si>
+  <si>
+    <t>9331826999</t>
+  </si>
+  <si>
+    <t>tran1949000251</t>
+  </si>
+  <si>
+    <t>transaction11949000251</t>
+  </si>
+  <si>
+    <t>2118214867</t>
+  </si>
+  <si>
+    <t>6497937328</t>
+  </si>
+  <si>
+    <t>tran8997507949</t>
+  </si>
+  <si>
+    <t>transaction18997507949</t>
+  </si>
+  <si>
+    <t>7625847128</t>
+  </si>
+  <si>
+    <t>6994520570</t>
+  </si>
+  <si>
+    <t>tran4425098945</t>
+  </si>
+  <si>
+    <t>transaction14425098945</t>
+  </si>
+  <si>
+    <t>2842644718</t>
+  </si>
+  <si>
+    <t>2243923045</t>
+  </si>
+  <si>
+    <t>tran1293955283</t>
+  </si>
+  <si>
+    <t>transaction11293955283</t>
+  </si>
+  <si>
+    <t>2766941428</t>
+  </si>
+  <si>
+    <t>4216622342</t>
+  </si>
+  <si>
+    <t>tran2549229582</t>
+  </si>
+  <si>
+    <t>transaction12549229582</t>
+  </si>
+  <si>
+    <t>1457250196</t>
+  </si>
+  <si>
+    <t>3760292130</t>
+  </si>
+  <si>
+    <t>tran2536755687</t>
+  </si>
+  <si>
+    <t>transaction12536755687</t>
+  </si>
+  <si>
+    <t>5075945679</t>
+  </si>
+  <si>
+    <t>9744662006</t>
+  </si>
+  <si>
+    <t>tran2378589597</t>
+  </si>
+  <si>
+    <t>transaction12378589597</t>
+  </si>
+  <si>
+    <t>1535314849</t>
+  </si>
+  <si>
+    <t>8279352725</t>
+  </si>
+  <si>
+    <t>tran3440607865</t>
+  </si>
+  <si>
+    <t>transaction13440607865</t>
+  </si>
+  <si>
+    <t>4682582540</t>
+  </si>
+  <si>
+    <t>8139240970</t>
+  </si>
+  <si>
+    <t>tran2433859098</t>
+  </si>
+  <si>
+    <t>transaction12433859098</t>
+  </si>
+  <si>
+    <t>2808088870</t>
+  </si>
+  <si>
+    <t>5173815420</t>
+  </si>
+  <si>
+    <t>tran7453183313</t>
+  </si>
+  <si>
+    <t>transaction17453183313</t>
+  </si>
+  <si>
+    <t>1670309718</t>
+  </si>
+  <si>
+    <t>4750749415</t>
+  </si>
+  <si>
+    <t>tran3299406036</t>
+  </si>
+  <si>
+    <t>transaction13299406036</t>
+  </si>
+  <si>
+    <t>7253264713</t>
+  </si>
+  <si>
+    <t>4736397638</t>
+  </si>
+  <si>
+    <t>tran7067842719</t>
+  </si>
+  <si>
+    <t>transaction17067842719</t>
+  </si>
+  <si>
+    <t>8060856041</t>
+  </si>
+  <si>
+    <t>8258274503</t>
+  </si>
+  <si>
+    <t>tran5755709358</t>
+  </si>
+  <si>
+    <t>transaction15755709358</t>
+  </si>
+  <si>
+    <t>5350281757</t>
+  </si>
+  <si>
+    <t>3175250572</t>
+  </si>
+  <si>
+    <t>tran8464047390</t>
+  </si>
+  <si>
+    <t>transaction18464047390</t>
+  </si>
+  <si>
+    <t>8295590078</t>
+  </si>
+  <si>
+    <t>7327582220</t>
+  </si>
+  <si>
+    <t>tran3763034645</t>
+  </si>
+  <si>
+    <t>transaction13763034645</t>
+  </si>
+  <si>
+    <t>4181866389</t>
+  </si>
+  <si>
+    <t>7729145111</t>
+  </si>
+  <si>
+    <t>tran8688209546</t>
+  </si>
+  <si>
+    <t>transaction18688209546</t>
+  </si>
+  <si>
+    <t>1716831963</t>
+  </si>
+  <si>
+    <t>6607326096</t>
+  </si>
+  <si>
+    <t>tran1982921143</t>
+  </si>
+  <si>
+    <t>transaction11982921143</t>
+  </si>
+  <si>
+    <t>tran4388874321</t>
+  </si>
+  <si>
+    <t>transaction14388874321</t>
+  </si>
+  <si>
+    <t>tran9365374312</t>
+  </si>
+  <si>
+    <t>transaction19365374312</t>
+  </si>
+  <si>
+    <t>tran6487817662</t>
+  </si>
+  <si>
+    <t>transaction16487817662</t>
+  </si>
+  <si>
+    <t>tran3733296319</t>
+  </si>
+  <si>
+    <t>transaction13733296319</t>
+  </si>
+  <si>
+    <t>tran7909879063</t>
+  </si>
+  <si>
+    <t>transaction17909879063</t>
+  </si>
+  <si>
+    <t>tran3554406136</t>
+  </si>
+  <si>
+    <t>transaction13554406136</t>
+  </si>
+  <si>
+    <t>tran8777306725</t>
+  </si>
+  <si>
+    <t>transaction18777306725</t>
+  </si>
+  <si>
+    <t>1466443356</t>
+  </si>
+  <si>
+    <t>9854716055</t>
   </si>
 </sst>
 </file>
@@ -2382,7 +2937,7 @@
   <dimension ref="A1:CS3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -2773,10 +3328,10 @@
     </row>
     <row r="2" spans="1:97" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>652</v>
+        <v>837</v>
       </c>
       <c r="B2" t="s">
-        <v>654</v>
+        <v>839</v>
       </c>
       <c r="C2" t="s">
         <v>488</v>
@@ -2785,7 +3340,7 @@
         <v>233</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="F2" t="s">
         <v>97</v>
@@ -2803,7 +3358,7 @@
         <v>97</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="L2" t="s">
         <v>97</v>
@@ -2848,7 +3403,7 @@
         <v>100</v>
       </c>
       <c r="Z2" s="1" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="AA2" t="s">
         <v>97</v>
@@ -2861,7 +3416,7 @@
       </c>
       <c r="AD2" s="2"/>
       <c r="AE2" s="1" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="AF2" t="s">
         <v>97</v>
@@ -2882,10 +3437,10 @@
         <v>97</v>
       </c>
       <c r="AL2" s="1" t="s">
+        <v>647</v>
+      </c>
+      <c r="AM2" s="1" t="s">
         <v>648</v>
-      </c>
-      <c r="AM2" s="1" t="s">
-        <v>649</v>
       </c>
       <c r="AN2" s="3" t="s">
         <v>488</v>
@@ -3020,7 +3575,7 @@
         <v>97</v>
       </c>
       <c r="CP2" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="CQ2" t="s">
         <v>97</v>
@@ -3034,10 +3589,10 @@
     </row>
     <row r="3" spans="1:97" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>653</v>
+        <v>838</v>
       </c>
       <c r="B3" t="s">
-        <v>655</v>
+        <v>840</v>
       </c>
       <c r="C3" t="s">
         <v>488</v>
@@ -3046,10 +3601,10 @@
         <v>233</v>
       </c>
       <c r="E3" s="1" t="s">
+        <v>643</v>
+      </c>
+      <c r="K3" s="1" t="s">
         <v>644</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>645</v>
       </c>
       <c r="S3" s="1" t="s">
         <v>132</v>
@@ -3061,7 +3616,7 @@
         <v>100</v>
       </c>
       <c r="Z3" s="1" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="AB3" s="1" t="s">
         <v>141</v>
@@ -3071,13 +3626,13 @@
       </c>
       <c r="AD3" s="2"/>
       <c r="AE3" s="1" t="s">
+        <v>646</v>
+      </c>
+      <c r="AL3" s="1" t="s">
         <v>647</v>
       </c>
-      <c r="AL3" s="1" t="s">
+      <c r="AM3" s="1" t="s">
         <v>648</v>
-      </c>
-      <c r="AM3" s="1" t="s">
-        <v>649</v>
       </c>
       <c r="AN3" s="3" t="s">
         <v>488</v>
@@ -3107,7 +3662,7 @@
         <v>632</v>
       </c>
       <c r="CP3" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
change schedule at time
</commit_message>
<xml_diff>
--- a/src/main/resources/Bulk_ConventionalTransactions_File.xlsx
+++ b/src/main/resources/Bulk_ConventionalTransactions_File.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24593" uniqueCount="841">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24422" uniqueCount="679">
   <si>
     <t>transactionName</t>
   </si>
@@ -1960,589 +1960,103 @@
     <t>SCBLINBB</t>
   </si>
   <si>
-    <t>ACCRAK1</t>
-  </si>
-  <si>
     <t>ADD1</t>
   </si>
   <si>
     <t>ADD2</t>
   </si>
   <si>
-    <t>tran31562851993</t>
+    <t>ACCRAK132</t>
   </si>
   <si>
-    <t>transaction131563285199</t>
+    <t>ACCRAK1867</t>
   </si>
   <si>
-    <t>tran2220410189</t>
+    <t>tran2824492469</t>
   </si>
   <si>
-    <t>transaction12220410189</t>
+    <t>transaction12824492469</t>
   </si>
   <si>
-    <t>5926839309</t>
+    <t>8188244029</t>
   </si>
   <si>
-    <t>1917075353</t>
+    <t>1987511998</t>
   </si>
   <si>
-    <t>tran3168975030</t>
+    <t>tran4900991552</t>
   </si>
   <si>
-    <t>transaction13168975030</t>
+    <t>transaction14900991552</t>
   </si>
   <si>
-    <t>9720385224</t>
+    <t>9053892786</t>
   </si>
   <si>
-    <t>2869605032</t>
+    <t>1872364902</t>
   </si>
   <si>
-    <t>tran2675526863</t>
+    <t>11.37 AM</t>
   </si>
   <si>
-    <t>transaction12675526863</t>
+    <t>tran5751985401</t>
   </si>
   <si>
-    <t>1360284043</t>
+    <t>transaction15751985401</t>
   </si>
   <si>
-    <t>6692107930</t>
+    <t>2553774071</t>
   </si>
   <si>
-    <t>tran4563878273</t>
+    <t>4814091974</t>
   </si>
   <si>
-    <t>transaction14563878273</t>
+    <t>12.18 PM</t>
   </si>
   <si>
-    <t>2174591355</t>
+    <t>tran6515111970</t>
   </si>
   <si>
-    <t>8397647418</t>
+    <t>transaction16515111970</t>
   </si>
   <si>
-    <t>tran2536298242</t>
+    <t>7846345842</t>
   </si>
   <si>
-    <t>transaction12536298242</t>
+    <t>5212267249</t>
   </si>
   <si>
-    <t>7201670404</t>
+    <t>12.57 PM</t>
   </si>
   <si>
-    <t>3606527842</t>
+    <t>tran4260025472</t>
   </si>
   <si>
-    <t>tran6018555551</t>
+    <t>transaction14260025472</t>
   </si>
   <si>
-    <t>transaction16018555551</t>
+    <t>2222959970</t>
   </si>
   <si>
-    <t>4080447587</t>
+    <t>4169697419</t>
   </si>
   <si>
-    <t>4554549065</t>
+    <t>01.05 PM</t>
   </si>
   <si>
-    <t>tran4810984332</t>
+    <t>tran2961849940</t>
   </si>
   <si>
-    <t>transaction14810984332</t>
+    <t>transaction12961849940</t>
   </si>
   <si>
-    <t>4353486664</t>
+    <t>5968735885</t>
   </si>
   <si>
-    <t>9631293769</t>
+    <t>2709705659</t>
   </si>
   <si>
-    <t>tran1033549629</t>
-  </si>
-  <si>
-    <t>transaction11033549629</t>
-  </si>
-  <si>
-    <t>7875127720</t>
-  </si>
-  <si>
-    <t>3203268155</t>
-  </si>
-  <si>
-    <t>tran4386579392</t>
-  </si>
-  <si>
-    <t>transaction14386579392</t>
-  </si>
-  <si>
-    <t>2188908755</t>
-  </si>
-  <si>
-    <t>1749649300</t>
-  </si>
-  <si>
-    <t>tran4547006125</t>
-  </si>
-  <si>
-    <t>transaction14547006125</t>
-  </si>
-  <si>
-    <t>2189716657</t>
-  </si>
-  <si>
-    <t>6689142101</t>
-  </si>
-  <si>
-    <t>tran1242020376</t>
-  </si>
-  <si>
-    <t>transaction11242020376</t>
-  </si>
-  <si>
-    <t>9648715418</t>
-  </si>
-  <si>
-    <t>3309382468</t>
-  </si>
-  <si>
-    <t>tran9878986976</t>
-  </si>
-  <si>
-    <t>transaction19878986976</t>
-  </si>
-  <si>
-    <t>6804857608</t>
-  </si>
-  <si>
-    <t>6054139799</t>
-  </si>
-  <si>
-    <t>tran7084720137</t>
-  </si>
-  <si>
-    <t>transaction17084720137</t>
-  </si>
-  <si>
-    <t>7595892522</t>
-  </si>
-  <si>
-    <t>6646597229</t>
-  </si>
-  <si>
-    <t>tran2798396314</t>
-  </si>
-  <si>
-    <t>transaction12798396314</t>
-  </si>
-  <si>
-    <t>5927640401</t>
-  </si>
-  <si>
-    <t>1574612081</t>
-  </si>
-  <si>
-    <t>tran7420727064</t>
-  </si>
-  <si>
-    <t>transaction17420727064</t>
-  </si>
-  <si>
-    <t>4854969548</t>
-  </si>
-  <si>
-    <t>7337787878</t>
-  </si>
-  <si>
-    <t>tran7454406510</t>
-  </si>
-  <si>
-    <t>transaction17454406510</t>
-  </si>
-  <si>
-    <t>7415668699</t>
-  </si>
-  <si>
-    <t>7185795517</t>
-  </si>
-  <si>
-    <t>tran8736375407</t>
-  </si>
-  <si>
-    <t>transaction18736375407</t>
-  </si>
-  <si>
-    <t>7332437496</t>
-  </si>
-  <si>
-    <t>8739602199</t>
-  </si>
-  <si>
-    <t>tran7853762411</t>
-  </si>
-  <si>
-    <t>transaction17853762411</t>
-  </si>
-  <si>
-    <t>7622005242</t>
-  </si>
-  <si>
-    <t>6947382697</t>
-  </si>
-  <si>
-    <t>tran1897754676</t>
-  </si>
-  <si>
-    <t>transaction11897754676</t>
-  </si>
-  <si>
-    <t>7237888936</t>
-  </si>
-  <si>
-    <t>8607114659</t>
-  </si>
-  <si>
-    <t>tran4895374326</t>
-  </si>
-  <si>
-    <t>transaction14895374326</t>
-  </si>
-  <si>
-    <t>3006292919</t>
-  </si>
-  <si>
-    <t>2499900981</t>
-  </si>
-  <si>
-    <t>tran5462140886</t>
-  </si>
-  <si>
-    <t>transaction15462140886</t>
-  </si>
-  <si>
-    <t>2539719545</t>
-  </si>
-  <si>
-    <t>9883845829</t>
-  </si>
-  <si>
-    <t>tran2862118519</t>
-  </si>
-  <si>
-    <t>transaction12862118519</t>
-  </si>
-  <si>
-    <t>5355501345</t>
-  </si>
-  <si>
-    <t>4151484857</t>
-  </si>
-  <si>
-    <t>tran5827868989</t>
-  </si>
-  <si>
-    <t>transaction15827868989</t>
-  </si>
-  <si>
-    <t>7345037513</t>
-  </si>
-  <si>
-    <t>7643266198</t>
-  </si>
-  <si>
-    <t>tran1942908760</t>
-  </si>
-  <si>
-    <t>transaction11942908760</t>
-  </si>
-  <si>
-    <t>1122062616</t>
-  </si>
-  <si>
-    <t>6050676410</t>
-  </si>
-  <si>
-    <t>tran7785455375</t>
-  </si>
-  <si>
-    <t>transaction17785455375</t>
-  </si>
-  <si>
-    <t>1160598615</t>
-  </si>
-  <si>
-    <t>5601738662</t>
-  </si>
-  <si>
-    <t>tran7329995884</t>
-  </si>
-  <si>
-    <t>transaction17329995884</t>
-  </si>
-  <si>
-    <t>1357910765</t>
-  </si>
-  <si>
-    <t>2709621822</t>
-  </si>
-  <si>
-    <t>tran7778548431</t>
-  </si>
-  <si>
-    <t>transaction17778548431</t>
-  </si>
-  <si>
-    <t>8439142179</t>
-  </si>
-  <si>
-    <t>9331826999</t>
-  </si>
-  <si>
-    <t>tran1949000251</t>
-  </si>
-  <si>
-    <t>transaction11949000251</t>
-  </si>
-  <si>
-    <t>2118214867</t>
-  </si>
-  <si>
-    <t>6497937328</t>
-  </si>
-  <si>
-    <t>tran8997507949</t>
-  </si>
-  <si>
-    <t>transaction18997507949</t>
-  </si>
-  <si>
-    <t>7625847128</t>
-  </si>
-  <si>
-    <t>6994520570</t>
-  </si>
-  <si>
-    <t>tran4425098945</t>
-  </si>
-  <si>
-    <t>transaction14425098945</t>
-  </si>
-  <si>
-    <t>2842644718</t>
-  </si>
-  <si>
-    <t>2243923045</t>
-  </si>
-  <si>
-    <t>tran1293955283</t>
-  </si>
-  <si>
-    <t>transaction11293955283</t>
-  </si>
-  <si>
-    <t>2766941428</t>
-  </si>
-  <si>
-    <t>4216622342</t>
-  </si>
-  <si>
-    <t>tran2549229582</t>
-  </si>
-  <si>
-    <t>transaction12549229582</t>
-  </si>
-  <si>
-    <t>1457250196</t>
-  </si>
-  <si>
-    <t>3760292130</t>
-  </si>
-  <si>
-    <t>tran2536755687</t>
-  </si>
-  <si>
-    <t>transaction12536755687</t>
-  </si>
-  <si>
-    <t>5075945679</t>
-  </si>
-  <si>
-    <t>9744662006</t>
-  </si>
-  <si>
-    <t>tran2378589597</t>
-  </si>
-  <si>
-    <t>transaction12378589597</t>
-  </si>
-  <si>
-    <t>1535314849</t>
-  </si>
-  <si>
-    <t>8279352725</t>
-  </si>
-  <si>
-    <t>tran3440607865</t>
-  </si>
-  <si>
-    <t>transaction13440607865</t>
-  </si>
-  <si>
-    <t>4682582540</t>
-  </si>
-  <si>
-    <t>8139240970</t>
-  </si>
-  <si>
-    <t>tran2433859098</t>
-  </si>
-  <si>
-    <t>transaction12433859098</t>
-  </si>
-  <si>
-    <t>2808088870</t>
-  </si>
-  <si>
-    <t>5173815420</t>
-  </si>
-  <si>
-    <t>tran7453183313</t>
-  </si>
-  <si>
-    <t>transaction17453183313</t>
-  </si>
-  <si>
-    <t>1670309718</t>
-  </si>
-  <si>
-    <t>4750749415</t>
-  </si>
-  <si>
-    <t>tran3299406036</t>
-  </si>
-  <si>
-    <t>transaction13299406036</t>
-  </si>
-  <si>
-    <t>7253264713</t>
-  </si>
-  <si>
-    <t>4736397638</t>
-  </si>
-  <si>
-    <t>tran7067842719</t>
-  </si>
-  <si>
-    <t>transaction17067842719</t>
-  </si>
-  <si>
-    <t>8060856041</t>
-  </si>
-  <si>
-    <t>8258274503</t>
-  </si>
-  <si>
-    <t>tran5755709358</t>
-  </si>
-  <si>
-    <t>transaction15755709358</t>
-  </si>
-  <si>
-    <t>5350281757</t>
-  </si>
-  <si>
-    <t>3175250572</t>
-  </si>
-  <si>
-    <t>tran8464047390</t>
-  </si>
-  <si>
-    <t>transaction18464047390</t>
-  </si>
-  <si>
-    <t>8295590078</t>
-  </si>
-  <si>
-    <t>7327582220</t>
-  </si>
-  <si>
-    <t>tran3763034645</t>
-  </si>
-  <si>
-    <t>transaction13763034645</t>
-  </si>
-  <si>
-    <t>4181866389</t>
-  </si>
-  <si>
-    <t>7729145111</t>
-  </si>
-  <si>
-    <t>tran8688209546</t>
-  </si>
-  <si>
-    <t>transaction18688209546</t>
-  </si>
-  <si>
-    <t>1716831963</t>
-  </si>
-  <si>
-    <t>6607326096</t>
-  </si>
-  <si>
-    <t>tran1982921143</t>
-  </si>
-  <si>
-    <t>transaction11982921143</t>
-  </si>
-  <si>
-    <t>tran4388874321</t>
-  </si>
-  <si>
-    <t>transaction14388874321</t>
-  </si>
-  <si>
-    <t>tran9365374312</t>
-  </si>
-  <si>
-    <t>transaction19365374312</t>
-  </si>
-  <si>
-    <t>tran6487817662</t>
-  </si>
-  <si>
-    <t>transaction16487817662</t>
-  </si>
-  <si>
-    <t>tran3733296319</t>
-  </si>
-  <si>
-    <t>transaction13733296319</t>
-  </si>
-  <si>
-    <t>tran7909879063</t>
-  </si>
-  <si>
-    <t>transaction17909879063</t>
-  </si>
-  <si>
-    <t>tran3554406136</t>
-  </si>
-  <si>
-    <t>transaction13554406136</t>
-  </si>
-  <si>
-    <t>tran8777306725</t>
-  </si>
-  <si>
-    <t>transaction18777306725</t>
-  </si>
-  <si>
-    <t>1466443356</t>
-  </si>
-  <si>
-    <t>9854716055</t>
+    <t>01.16 PM</t>
   </si>
 </sst>
 </file>
@@ -2936,8 +2450,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CS3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="V1" sqref="V1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -2961,7 +2475,7 @@
     <col min="18" max="18" bestFit="true" customWidth="true" width="17.3984375" collapsed="true"/>
     <col min="19" max="19" bestFit="true" customWidth="true" width="17.796875" collapsed="true"/>
     <col min="20" max="20" bestFit="true" customWidth="true" width="9.796875" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" width="10.19921875" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" width="13.19921875" collapsed="true"/>
     <col min="22" max="22" bestFit="true" customWidth="true" width="12.3984375" collapsed="true"/>
     <col min="23" max="23" bestFit="true" customWidth="true" width="12.5" collapsed="true"/>
     <col min="24" max="24" bestFit="true" customWidth="true" width="10.19921875" collapsed="true"/>
@@ -2971,7 +2485,7 @@
     <col min="28" max="28" bestFit="true" customWidth="true" width="15.09765625" collapsed="true"/>
     <col min="29" max="29" bestFit="true" customWidth="true" width="15.59765625" collapsed="true"/>
     <col min="30" max="30" bestFit="true" customWidth="true" width="9.59765625" collapsed="true"/>
-    <col min="31" max="31" bestFit="true" customWidth="true" width="8.59765625" collapsed="true"/>
+    <col min="31" max="31" bestFit="true" customWidth="true" width="11.59765625" collapsed="true"/>
     <col min="32" max="32" bestFit="true" customWidth="true" width="11.69921875" collapsed="true"/>
     <col min="33" max="33" bestFit="true" customWidth="true" width="18.296875" collapsed="true"/>
     <col min="34" max="34" bestFit="true" customWidth="true" width="15.09765625" collapsed="true"/>
@@ -3328,10 +2842,10 @@
     </row>
     <row r="2" spans="1:97" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>837</v>
+        <v>674</v>
       </c>
       <c r="B2" t="s">
-        <v>839</v>
+        <v>676</v>
       </c>
       <c r="C2" t="s">
         <v>488</v>
@@ -3388,10 +2902,10 @@
         <v>97</v>
       </c>
       <c r="U2" t="s">
-        <v>97</v>
+        <v>109</v>
       </c>
       <c r="V2" t="s">
-        <v>97</v>
+        <v>678</v>
       </c>
       <c r="W2" s="1" t="s">
         <v>103</v>
@@ -3416,7 +2930,7 @@
       </c>
       <c r="AD2" s="2"/>
       <c r="AE2" s="1" t="s">
-        <v>646</v>
+        <v>649</v>
       </c>
       <c r="AF2" t="s">
         <v>97</v>
@@ -3437,10 +2951,10 @@
         <v>97</v>
       </c>
       <c r="AL2" s="1" t="s">
+        <v>646</v>
+      </c>
+      <c r="AM2" s="1" t="s">
         <v>647</v>
-      </c>
-      <c r="AM2" s="1" t="s">
-        <v>648</v>
       </c>
       <c r="AN2" s="3" t="s">
         <v>488</v>
@@ -3589,10 +3103,10 @@
     </row>
     <row r="3" spans="1:97" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>838</v>
+        <v>675</v>
       </c>
       <c r="B3" t="s">
-        <v>840</v>
+        <v>677</v>
       </c>
       <c r="C3" t="s">
         <v>488</v>
@@ -3609,6 +3123,12 @@
       <c r="S3" s="1" t="s">
         <v>132</v>
       </c>
+      <c r="U3" t="s">
+        <v>109</v>
+      </c>
+      <c r="V3" t="s">
+        <v>678</v>
+      </c>
       <c r="W3" s="1" t="s">
         <v>103</v>
       </c>
@@ -3626,13 +3146,13 @@
       </c>
       <c r="AD3" s="2"/>
       <c r="AE3" s="1" t="s">
+        <v>648</v>
+      </c>
+      <c r="AL3" s="1" t="s">
         <v>646</v>
       </c>
-      <c r="AL3" s="1" t="s">
+      <c r="AM3" s="1" t="s">
         <v>647</v>
-      </c>
-      <c r="AM3" s="1" t="s">
-        <v>648</v>
       </c>
       <c r="AN3" s="3" t="s">
         <v>488</v>
@@ -3669,7 +3189,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:J1 F2:J2 L1:CS1 L2:R2 T2:V2 X2 AA2 AF2:AK2 BE2:BR2 BT2 BV2:CO2 CQ2:CS2" numberStoredAsText="1"/>
+    <ignoredError sqref="A1:J1 F2:J2 L1:U1 L2:R2 T2 X2 AA2 AF2:AK2 BE2:BR2 BT2 BV2:CO2 CQ2:CS2 V2 W1:CS1" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -3679,7 +3199,7 @@
   <dimension ref="A1:IQ306"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -77089,7 +76609,7 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:IQ306" numberStoredAsText="1"/>
+    <ignoredError sqref="A1:IQ4 A6:IQ306 A5:C5 E5:IQ5" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
iterate all report status
</commit_message>
<xml_diff>
--- a/src/main/resources/Bulk_ConventionalTransactions_File.xlsx
+++ b/src/main/resources/Bulk_ConventionalTransactions_File.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24422" uniqueCount="679">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24458" uniqueCount="709">
   <si>
     <t>transactionName</t>
   </si>
@@ -2058,6 +2058,96 @@
   <si>
     <t>01.16 PM</t>
   </si>
+  <si>
+    <t>tran4965433832</t>
+  </si>
+  <si>
+    <t>transaction14965433832</t>
+  </si>
+  <si>
+    <t>8037772175</t>
+  </si>
+  <si>
+    <t>8046481903</t>
+  </si>
+  <si>
+    <t>02.35 PM</t>
+  </si>
+  <si>
+    <t>tran7083747862</t>
+  </si>
+  <si>
+    <t>transaction17083747862</t>
+  </si>
+  <si>
+    <t>8382692307</t>
+  </si>
+  <si>
+    <t>3679862499</t>
+  </si>
+  <si>
+    <t>03.51 PM</t>
+  </si>
+  <si>
+    <t>tran3800447970</t>
+  </si>
+  <si>
+    <t>transaction13800447970</t>
+  </si>
+  <si>
+    <t>1927934092</t>
+  </si>
+  <si>
+    <t>3163916840</t>
+  </si>
+  <si>
+    <t>04.05 PM</t>
+  </si>
+  <si>
+    <t>tran9609146007</t>
+  </si>
+  <si>
+    <t>transaction19609146007</t>
+  </si>
+  <si>
+    <t>1444715759</t>
+  </si>
+  <si>
+    <t>3099884742</t>
+  </si>
+  <si>
+    <t>04.08 PM</t>
+  </si>
+  <si>
+    <t>tran4598281393</t>
+  </si>
+  <si>
+    <t>transaction14598281393</t>
+  </si>
+  <si>
+    <t>3865389061</t>
+  </si>
+  <si>
+    <t>9591483918</t>
+  </si>
+  <si>
+    <t>05.46 PM</t>
+  </si>
+  <si>
+    <t>tran2067055416</t>
+  </si>
+  <si>
+    <t>transaction12067055416</t>
+  </si>
+  <si>
+    <t>2310048982</t>
+  </si>
+  <si>
+    <t>7211318695</t>
+  </si>
+  <si>
+    <t>05.58 PM</t>
+  </si>
 </sst>
 </file>
 
@@ -2842,10 +2932,10 @@
     </row>
     <row r="2" spans="1:97" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>674</v>
+        <v>704</v>
       </c>
       <c r="B2" t="s">
-        <v>676</v>
+        <v>706</v>
       </c>
       <c r="C2" t="s">
         <v>488</v>
@@ -2905,7 +2995,7 @@
         <v>109</v>
       </c>
       <c r="V2" t="s">
-        <v>678</v>
+        <v>708</v>
       </c>
       <c r="W2" s="1" t="s">
         <v>103</v>
@@ -3103,10 +3193,10 @@
     </row>
     <row r="3" spans="1:97" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>675</v>
+        <v>705</v>
       </c>
       <c r="B3" t="s">
-        <v>677</v>
+        <v>707</v>
       </c>
       <c r="C3" t="s">
         <v>488</v>
@@ -3127,7 +3217,7 @@
         <v>109</v>
       </c>
       <c r="V3" t="s">
-        <v>678</v>
+        <v>708</v>
       </c>
       <c r="W3" s="1" t="s">
         <v>103</v>

</xml_diff>

<commit_message>
change the xpath deal id search in report
</commit_message>
<xml_diff>
--- a/src/main/resources/Bulk_ConventionalTransactions_File.xlsx
+++ b/src/main/resources/Bulk_ConventionalTransactions_File.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24464" uniqueCount="714">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24482" uniqueCount="729">
   <si>
     <t>transactionName</t>
   </si>
@@ -2163,6 +2163,51 @@
   <si>
     <t>10.16 AM</t>
   </si>
+  <si>
+    <t>tran8231494953</t>
+  </si>
+  <si>
+    <t>transaction18231494953</t>
+  </si>
+  <si>
+    <t>2977110997</t>
+  </si>
+  <si>
+    <t>1574214716</t>
+  </si>
+  <si>
+    <t>05.00 PM</t>
+  </si>
+  <si>
+    <t>tran2035892075</t>
+  </si>
+  <si>
+    <t>transaction12035892075</t>
+  </si>
+  <si>
+    <t>3796723388</t>
+  </si>
+  <si>
+    <t>9236412898</t>
+  </si>
+  <si>
+    <t>05.29 PM</t>
+  </si>
+  <si>
+    <t>tran5002980012</t>
+  </si>
+  <si>
+    <t>transaction15002980012</t>
+  </si>
+  <si>
+    <t>8099308384</t>
+  </si>
+  <si>
+    <t>8142655474</t>
+  </si>
+  <si>
+    <t>05.54 PM</t>
+  </si>
 </sst>
 </file>
 
@@ -2947,10 +2992,10 @@
     </row>
     <row r="2" spans="1:97" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>709</v>
+        <v>724</v>
       </c>
       <c r="B2" t="s">
-        <v>711</v>
+        <v>726</v>
       </c>
       <c r="C2" t="s">
         <v>488</v>
@@ -3010,7 +3055,7 @@
         <v>109</v>
       </c>
       <c r="V2" t="s">
-        <v>713</v>
+        <v>728</v>
       </c>
       <c r="W2" s="1" t="s">
         <v>103</v>
@@ -3208,10 +3253,10 @@
     </row>
     <row r="3" spans="1:97" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>710</v>
+        <v>725</v>
       </c>
       <c r="B3" t="s">
-        <v>712</v>
+        <v>727</v>
       </c>
       <c r="C3" t="s">
         <v>488</v>
@@ -3232,7 +3277,7 @@
         <v>109</v>
       </c>
       <c r="V3" t="s">
-        <v>713</v>
+        <v>728</v>
       </c>
       <c r="W3" s="1" t="s">
         <v>103</v>

</xml_diff>

<commit_message>
Created Payload for static rule
</commit_message>
<xml_diff>
--- a/src/main/resources/Bulk_ConventionalTransactions_File.xlsx
+++ b/src/main/resources/Bulk_ConventionalTransactions_File.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24482" uniqueCount="729">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24488" uniqueCount="734">
   <si>
     <t>transactionName</t>
   </si>
@@ -2208,6 +2208,21 @@
   <si>
     <t>05.54 PM</t>
   </si>
+  <si>
+    <t>tran9239361074</t>
+  </si>
+  <si>
+    <t>transaction19239361074</t>
+  </si>
+  <si>
+    <t>3445476954</t>
+  </si>
+  <si>
+    <t>1413857195</t>
+  </si>
+  <si>
+    <t>04.23 PM</t>
+  </si>
 </sst>
 </file>
 
@@ -2992,10 +3007,10 @@
     </row>
     <row r="2" spans="1:97" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>724</v>
+        <v>729</v>
       </c>
       <c r="B2" t="s">
-        <v>726</v>
+        <v>731</v>
       </c>
       <c r="C2" t="s">
         <v>488</v>
@@ -3055,7 +3070,7 @@
         <v>109</v>
       </c>
       <c r="V2" t="s">
-        <v>728</v>
+        <v>733</v>
       </c>
       <c r="W2" s="1" t="s">
         <v>103</v>
@@ -3253,10 +3268,10 @@
     </row>
     <row r="3" spans="1:97" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>725</v>
+        <v>730</v>
       </c>
       <c r="B3" t="s">
-        <v>727</v>
+        <v>732</v>
       </c>
       <c r="C3" t="s">
         <v>488</v>
@@ -3277,7 +3292,7 @@
         <v>109</v>
       </c>
       <c r="V3" t="s">
-        <v>728</v>
+        <v>733</v>
       </c>
       <c r="W3" s="1" t="s">
         <v>103</v>

</xml_diff>

<commit_message>
changes made for failed test cases
</commit_message>
<xml_diff>
--- a/src/main/resources/Bulk_ConventionalTransactions_File.xlsx
+++ b/src/main/resources/Bulk_ConventionalTransactions_File.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24488" uniqueCount="734">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24494" uniqueCount="739">
   <si>
     <t>transactionName</t>
   </si>
@@ -2223,6 +2223,21 @@
   <si>
     <t>04.23 PM</t>
   </si>
+  <si>
+    <t>tran4838950870</t>
+  </si>
+  <si>
+    <t>transaction14838950870</t>
+  </si>
+  <si>
+    <t>6230055771</t>
+  </si>
+  <si>
+    <t>4028631016</t>
+  </si>
+  <si>
+    <t>02.50 PM</t>
+  </si>
 </sst>
 </file>
 
@@ -3007,10 +3022,10 @@
     </row>
     <row r="2" spans="1:97" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>729</v>
+        <v>734</v>
       </c>
       <c r="B2" t="s">
-        <v>731</v>
+        <v>736</v>
       </c>
       <c r="C2" t="s">
         <v>488</v>
@@ -3070,7 +3085,7 @@
         <v>109</v>
       </c>
       <c r="V2" t="s">
-        <v>733</v>
+        <v>738</v>
       </c>
       <c r="W2" s="1" t="s">
         <v>103</v>
@@ -3268,10 +3283,10 @@
     </row>
     <row r="3" spans="1:97" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>730</v>
+        <v>735</v>
       </c>
       <c r="B3" t="s">
-        <v>732</v>
+        <v>737</v>
       </c>
       <c r="C3" t="s">
         <v>488</v>
@@ -3292,7 +3307,7 @@
         <v>109</v>
       </c>
       <c r="V3" t="s">
-        <v>733</v>
+        <v>738</v>
       </c>
       <c r="W3" s="1" t="s">
         <v>103</v>

</xml_diff>

<commit_message>
checking failed test cases
</commit_message>
<xml_diff>
--- a/src/main/resources/Bulk_ConventionalTransactions_File.xlsx
+++ b/src/main/resources/Bulk_ConventionalTransactions_File.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24404" uniqueCount="664">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24410" uniqueCount="669">
   <si>
     <t>transactionName</t>
   </si>
@@ -2013,6 +2013,21 @@
   <si>
     <t>02.10 PM</t>
   </si>
+  <si>
+    <t>tran5152721115</t>
+  </si>
+  <si>
+    <t>transaction15152721115</t>
+  </si>
+  <si>
+    <t>3039610638</t>
+  </si>
+  <si>
+    <t>8854458970</t>
+  </si>
+  <si>
+    <t>05.20 PM</t>
+  </si>
 </sst>
 </file>
 
@@ -2797,10 +2812,10 @@
     </row>
     <row r="2" spans="1:97" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>659</v>
+        <v>664</v>
       </c>
       <c r="B2" t="s">
-        <v>661</v>
+        <v>666</v>
       </c>
       <c r="C2" t="s">
         <v>488</v>
@@ -2860,7 +2875,7 @@
         <v>109</v>
       </c>
       <c r="V2" t="s">
-        <v>663</v>
+        <v>668</v>
       </c>
       <c r="W2" s="1" t="s">
         <v>103</v>
@@ -3058,10 +3073,10 @@
     </row>
     <row r="3" spans="1:97" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>660</v>
+        <v>665</v>
       </c>
       <c r="B3" t="s">
-        <v>662</v>
+        <v>667</v>
       </c>
       <c r="C3" t="s">
         <v>488</v>
@@ -3082,7 +3097,7 @@
         <v>109</v>
       </c>
       <c r="V3" t="s">
-        <v>663</v>
+        <v>668</v>
       </c>
       <c r="W3" s="1" t="s">
         <v>103</v>

</xml_diff>

<commit_message>
Updated test case 8
</commit_message>
<xml_diff>
--- a/src/main/resources/Bulk_ConventionalTransactions_File.xlsx
+++ b/src/main/resources/Bulk_ConventionalTransactions_File.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24422" uniqueCount="679">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24428" uniqueCount="684">
   <si>
     <t>transactionName</t>
   </si>
@@ -2058,6 +2058,21 @@
   <si>
     <t>03.31 PM</t>
   </si>
+  <si>
+    <t>tran2827906332</t>
+  </si>
+  <si>
+    <t>transaction12827906332</t>
+  </si>
+  <si>
+    <t>9763894014</t>
+  </si>
+  <si>
+    <t>1191312922</t>
+  </si>
+  <si>
+    <t>05.06 PM</t>
+  </si>
 </sst>
 </file>
 
@@ -2842,10 +2857,10 @@
     </row>
     <row r="2" spans="1:97" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>674</v>
+        <v>679</v>
       </c>
       <c r="B2" t="s">
-        <v>676</v>
+        <v>681</v>
       </c>
       <c r="C2" t="s">
         <v>488</v>
@@ -2905,7 +2920,7 @@
         <v>109</v>
       </c>
       <c r="V2" t="s">
-        <v>678</v>
+        <v>683</v>
       </c>
       <c r="W2" s="1" t="s">
         <v>103</v>
@@ -3103,10 +3118,10 @@
     </row>
     <row r="3" spans="1:97" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>675</v>
+        <v>680</v>
       </c>
       <c r="B3" t="s">
-        <v>677</v>
+        <v>682</v>
       </c>
       <c r="C3" t="s">
         <v>488</v>
@@ -3127,7 +3142,7 @@
         <v>109</v>
       </c>
       <c r="V3" t="s">
-        <v>678</v>
+        <v>683</v>
       </c>
       <c r="W3" s="1" t="s">
         <v>103</v>

</xml_diff>

<commit_message>
Updated Failed test cases and Completed TS71,TS71_1
</commit_message>
<xml_diff>
--- a/src/main/resources/Bulk_ConventionalTransactions_File.xlsx
+++ b/src/main/resources/Bulk_ConventionalTransactions_File.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24458" uniqueCount="709">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24470" uniqueCount="719">
   <si>
     <t>transactionName</t>
   </si>
@@ -2148,6 +2148,36 @@
   <si>
     <t>12.19 PM</t>
   </si>
+  <si>
+    <t>tran5111109060</t>
+  </si>
+  <si>
+    <t>transaction15111109060</t>
+  </si>
+  <si>
+    <t>5152812000</t>
+  </si>
+  <si>
+    <t>1746833890</t>
+  </si>
+  <si>
+    <t>03.32 PM</t>
+  </si>
+  <si>
+    <t>tran4305968002</t>
+  </si>
+  <si>
+    <t>transaction14305968002</t>
+  </si>
+  <si>
+    <t>4651896915</t>
+  </si>
+  <si>
+    <t>5994509145</t>
+  </si>
+  <si>
+    <t>07.53 PM</t>
+  </si>
 </sst>
 </file>
 
@@ -2932,10 +2962,10 @@
     </row>
     <row r="2" spans="1:97" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>704</v>
+        <v>714</v>
       </c>
       <c r="B2" t="s">
-        <v>706</v>
+        <v>716</v>
       </c>
       <c r="C2" t="s">
         <v>488</v>
@@ -2995,7 +3025,7 @@
         <v>109</v>
       </c>
       <c r="V2" t="s">
-        <v>708</v>
+        <v>718</v>
       </c>
       <c r="W2" s="1" t="s">
         <v>103</v>
@@ -3193,10 +3223,10 @@
     </row>
     <row r="3" spans="1:97" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>705</v>
+        <v>715</v>
       </c>
       <c r="B3" t="s">
-        <v>707</v>
+        <v>717</v>
       </c>
       <c r="C3" t="s">
         <v>488</v>
@@ -3217,7 +3247,7 @@
         <v>109</v>
       </c>
       <c r="V3" t="s">
-        <v>708</v>
+        <v>718</v>
       </c>
       <c r="W3" s="1" t="s">
         <v>103</v>

</xml_diff>

<commit_message>
Updated failed test cases n started TS79
</commit_message>
<xml_diff>
--- a/src/main/resources/Bulk_ConventionalTransactions_File.xlsx
+++ b/src/main/resources/Bulk_ConventionalTransactions_File.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24578" uniqueCount="809">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24584" uniqueCount="814">
   <si>
     <t>transactionName</t>
   </si>
@@ -2447,6 +2447,21 @@
   </si>
   <si>
     <t>11.43 AM</t>
+  </si>
+  <si>
+    <t>tran2382787480</t>
+  </si>
+  <si>
+    <t>transaction12382787480</t>
+  </si>
+  <si>
+    <t>5604791330</t>
+  </si>
+  <si>
+    <t>6604400799</t>
+  </si>
+  <si>
+    <t>11.04 AM</t>
   </si>
 </sst>
 </file>
@@ -3232,10 +3247,10 @@
     </row>
     <row r="2" spans="1:97" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>804</v>
+        <v>809</v>
       </c>
       <c r="B2" t="s">
-        <v>806</v>
+        <v>811</v>
       </c>
       <c r="C2" t="s">
         <v>488</v>
@@ -3295,7 +3310,7 @@
         <v>109</v>
       </c>
       <c r="V2" t="s">
-        <v>808</v>
+        <v>813</v>
       </c>
       <c r="W2" s="1" t="s">
         <v>103</v>
@@ -3493,10 +3508,10 @@
     </row>
     <row r="3" spans="1:97" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>805</v>
+        <v>810</v>
       </c>
       <c r="B3" t="s">
-        <v>807</v>
+        <v>812</v>
       </c>
       <c r="C3" t="s">
         <v>488</v>
@@ -3517,7 +3532,7 @@
         <v>109</v>
       </c>
       <c r="V3" t="s">
-        <v>808</v>
+        <v>813</v>
       </c>
       <c r="W3" s="1" t="s">
         <v>103</v>

</xml_diff>

<commit_message>
Updated failed test cases and added TS81
</commit_message>
<xml_diff>
--- a/src/main/resources/Bulk_ConventionalTransactions_File.xlsx
+++ b/src/main/resources/Bulk_ConventionalTransactions_File.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24584" uniqueCount="814">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24602" uniqueCount="829">
   <si>
     <t>transactionName</t>
   </si>
@@ -2462,6 +2462,51 @@
   </si>
   <si>
     <t>11.04 AM</t>
+  </si>
+  <si>
+    <t>tran9373311504</t>
+  </si>
+  <si>
+    <t>transaction19373311504</t>
+  </si>
+  <si>
+    <t>2159935254</t>
+  </si>
+  <si>
+    <t>2881138817</t>
+  </si>
+  <si>
+    <t>10.34 AM</t>
+  </si>
+  <si>
+    <t>tran4721508959</t>
+  </si>
+  <si>
+    <t>transaction14721508959</t>
+  </si>
+  <si>
+    <t>1415468306</t>
+  </si>
+  <si>
+    <t>6823181159</t>
+  </si>
+  <si>
+    <t>11.33 AM</t>
+  </si>
+  <si>
+    <t>tran8003571414</t>
+  </si>
+  <si>
+    <t>transaction18003571414</t>
+  </si>
+  <si>
+    <t>7994782914</t>
+  </si>
+  <si>
+    <t>7283057670</t>
+  </si>
+  <si>
+    <t>10.14 AM</t>
   </si>
 </sst>
 </file>
@@ -3247,10 +3292,10 @@
     </row>
     <row r="2" spans="1:97" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>809</v>
+        <v>824</v>
       </c>
       <c r="B2" t="s">
-        <v>811</v>
+        <v>826</v>
       </c>
       <c r="C2" t="s">
         <v>488</v>
@@ -3310,7 +3355,7 @@
         <v>109</v>
       </c>
       <c r="V2" t="s">
-        <v>813</v>
+        <v>828</v>
       </c>
       <c r="W2" s="1" t="s">
         <v>103</v>
@@ -3508,10 +3553,10 @@
     </row>
     <row r="3" spans="1:97" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>810</v>
+        <v>825</v>
       </c>
       <c r="B3" t="s">
-        <v>812</v>
+        <v>827</v>
       </c>
       <c r="C3" t="s">
         <v>488</v>
@@ -3532,7 +3577,7 @@
         <v>109</v>
       </c>
       <c r="V3" t="s">
-        <v>813</v>
+        <v>828</v>
       </c>
       <c r="W3" s="1" t="s">
         <v>103</v>

</xml_diff>

<commit_message>
Updated test cases title
</commit_message>
<xml_diff>
--- a/src/main/resources/Bulk_ConventionalTransactions_File.xlsx
+++ b/src/main/resources/Bulk_ConventionalTransactions_File.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr codeName="ThisWorkbook"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\BDD_Framework\30 March\10MayNew\29May-Main\upp-test-automation\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\BDD_Framework\30 March\10MayNew\29May-Main\20 june\upp-test-automation\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24602" uniqueCount="829">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24393" uniqueCount="655">
   <si>
     <t>transactionName</t>
   </si>
@@ -1972,548 +1972,25 @@
     <t>ACCRAK1867</t>
   </si>
   <si>
-    <t>4876051439</t>
+    <t>8303135954</t>
   </si>
   <si>
-    <t>10.33 AM</t>
+    <t>5620312850</t>
   </si>
   <si>
-    <t>tran536153148082</t>
+    <t>12.17 PM</t>
   </si>
   <si>
-    <t>transaction1533615124808</t>
+    <t>tran9939963151c</t>
   </si>
   <si>
-    <t>tran1384680372</t>
-  </si>
-  <si>
-    <t>transaction11384680372</t>
-  </si>
-  <si>
-    <t>8237481903</t>
-  </si>
-  <si>
-    <t>9247444285</t>
-  </si>
-  <si>
-    <t>12.40 PM</t>
-  </si>
-  <si>
-    <t>tran1868649373</t>
-  </si>
-  <si>
-    <t>transaction11868649373</t>
-  </si>
-  <si>
-    <t>1633944618</t>
-  </si>
-  <si>
-    <t>4684871871</t>
-  </si>
-  <si>
-    <t>02.10 PM</t>
-  </si>
-  <si>
-    <t>tran5152721115</t>
-  </si>
-  <si>
-    <t>transaction15152721115</t>
-  </si>
-  <si>
-    <t>3039610638</t>
-  </si>
-  <si>
-    <t>8854458970</t>
-  </si>
-  <si>
-    <t>05.20 PM</t>
-  </si>
-  <si>
-    <t>tran6373677166</t>
-  </si>
-  <si>
-    <t>transaction16373677166</t>
-  </si>
-  <si>
-    <t>4250079331</t>
-  </si>
-  <si>
-    <t>5795406894</t>
-  </si>
-  <si>
-    <t>03.16 PM</t>
-  </si>
-  <si>
-    <t>tran3658364769</t>
-  </si>
-  <si>
-    <t>transaction13658364769</t>
-  </si>
-  <si>
-    <t>6200520733</t>
-  </si>
-  <si>
-    <t>9947174738</t>
-  </si>
-  <si>
-    <t>03.31 PM</t>
-  </si>
-  <si>
-    <t>tran2827906332</t>
-  </si>
-  <si>
-    <t>transaction12827906332</t>
-  </si>
-  <si>
-    <t>9763894014</t>
-  </si>
-  <si>
-    <t>1191312922</t>
-  </si>
-  <si>
-    <t>05.06 PM</t>
-  </si>
-  <si>
-    <t>tran5661430566</t>
-  </si>
-  <si>
-    <t>transaction15661430566</t>
-  </si>
-  <si>
-    <t>7618353438</t>
-  </si>
-  <si>
-    <t>5148955207</t>
-  </si>
-  <si>
-    <t>01.02 PM</t>
-  </si>
-  <si>
-    <t>tran1267609352</t>
-  </si>
-  <si>
-    <t>transaction11267609352</t>
-  </si>
-  <si>
-    <t>2499305197</t>
-  </si>
-  <si>
-    <t>6583338280</t>
-  </si>
-  <si>
-    <t>02.47 PM</t>
-  </si>
-  <si>
-    <t>tran2353546695</t>
-  </si>
-  <si>
-    <t>transaction12353546695</t>
-  </si>
-  <si>
-    <t>1455268256</t>
-  </si>
-  <si>
-    <t>9850492890</t>
-  </si>
-  <si>
-    <t>12.58 PM</t>
-  </si>
-  <si>
-    <t>tran4619476972</t>
-  </si>
-  <si>
-    <t>transaction14619476972</t>
-  </si>
-  <si>
-    <t>5714796331</t>
-  </si>
-  <si>
-    <t>8761306882</t>
-  </si>
-  <si>
-    <t>01.05 PM</t>
-  </si>
-  <si>
-    <t>tran3081676202</t>
-  </si>
-  <si>
-    <t>transaction13081676202</t>
-  </si>
-  <si>
-    <t>7813840297</t>
-  </si>
-  <si>
-    <t>5026866399</t>
-  </si>
-  <si>
-    <t>12.19 PM</t>
-  </si>
-  <si>
-    <t>tran5111109060</t>
-  </si>
-  <si>
-    <t>transaction15111109060</t>
-  </si>
-  <si>
-    <t>5152812000</t>
-  </si>
-  <si>
-    <t>1746833890</t>
-  </si>
-  <si>
-    <t>03.32 PM</t>
-  </si>
-  <si>
-    <t>tran4305968002</t>
-  </si>
-  <si>
-    <t>transaction14305968002</t>
-  </si>
-  <si>
-    <t>4651896915</t>
-  </si>
-  <si>
-    <t>5994509145</t>
-  </si>
-  <si>
-    <t>07.53 PM</t>
-  </si>
-  <si>
-    <t>tran1814398674</t>
-  </si>
-  <si>
-    <t>transaction11814398674</t>
-  </si>
-  <si>
-    <t>2221065187</t>
-  </si>
-  <si>
-    <t>3810708741</t>
-  </si>
-  <si>
-    <t>10.13 AM</t>
-  </si>
-  <si>
-    <t>tran1212681843</t>
-  </si>
-  <si>
-    <t>transaction11212681843</t>
-  </si>
-  <si>
-    <t>6485939943</t>
-  </si>
-  <si>
-    <t>4994725778</t>
-  </si>
-  <si>
-    <t>10.59 AM</t>
-  </si>
-  <si>
-    <t>tran4786681668</t>
-  </si>
-  <si>
-    <t>transaction14786681668</t>
-  </si>
-  <si>
-    <t>1032497236</t>
-  </si>
-  <si>
-    <t>1074177557</t>
-  </si>
-  <si>
-    <t>06.09 PM</t>
-  </si>
-  <si>
-    <t>tran2419430909</t>
-  </si>
-  <si>
-    <t>transaction12419430909</t>
-  </si>
-  <si>
-    <t>7489924704</t>
-  </si>
-  <si>
-    <t>7604891585</t>
-  </si>
-  <si>
-    <t>06.14 PM</t>
-  </si>
-  <si>
-    <t>tran3299737317</t>
-  </si>
-  <si>
-    <t>transaction13299737317</t>
-  </si>
-  <si>
-    <t>6998779814</t>
-  </si>
-  <si>
-    <t>4110280695</t>
-  </si>
-  <si>
-    <t>06.41 PM</t>
-  </si>
-  <si>
-    <t>tran9258117474</t>
-  </si>
-  <si>
-    <t>transaction19258117474</t>
-  </si>
-  <si>
-    <t>9683181354</t>
-  </si>
-  <si>
-    <t>9924125849</t>
-  </si>
-  <si>
-    <t>08.59 PM</t>
-  </si>
-  <si>
-    <t>tran2612885162</t>
-  </si>
-  <si>
-    <t>transaction12612885162</t>
-  </si>
-  <si>
-    <t>2046749162</t>
-  </si>
-  <si>
-    <t>1408690021</t>
-  </si>
-  <si>
-    <t>09.17 AM</t>
-  </si>
-  <si>
-    <t>tran6032764241</t>
-  </si>
-  <si>
-    <t>transaction16032764241</t>
-  </si>
-  <si>
-    <t>8621958347</t>
-  </si>
-  <si>
-    <t>5175890447</t>
-  </si>
-  <si>
-    <t>09.16 AM</t>
-  </si>
-  <si>
-    <t>tran6399319135</t>
-  </si>
-  <si>
-    <t>transaction16399319135</t>
-  </si>
-  <si>
-    <t>2044906161</t>
-  </si>
-  <si>
-    <t>4808014442</t>
-  </si>
-  <si>
-    <t>09.29 AM</t>
-  </si>
-  <si>
-    <t>tran6557266836</t>
-  </si>
-  <si>
-    <t>transaction16557266836</t>
-  </si>
-  <si>
-    <t>9642393071</t>
-  </si>
-  <si>
-    <t>6473095798</t>
-  </si>
-  <si>
-    <t>05.55 PM</t>
-  </si>
-  <si>
-    <t>tran7990262985</t>
-  </si>
-  <si>
-    <t>transaction17990262985</t>
-  </si>
-  <si>
-    <t>6484587207</t>
-  </si>
-  <si>
-    <t>2272643049</t>
-  </si>
-  <si>
-    <t>10.44 PM</t>
-  </si>
-  <si>
-    <t>tran1202360605</t>
-  </si>
-  <si>
-    <t>transaction11202360605</t>
-  </si>
-  <si>
-    <t>4659647671</t>
-  </si>
-  <si>
-    <t>1775680562</t>
-  </si>
-  <si>
-    <t>01.44 PM</t>
-  </si>
-  <si>
-    <t>tran5279098769</t>
-  </si>
-  <si>
-    <t>transaction15279098769</t>
-  </si>
-  <si>
-    <t>8651395565</t>
-  </si>
-  <si>
-    <t>5431273054</t>
-  </si>
-  <si>
-    <t>01.56 PM</t>
-  </si>
-  <si>
-    <t>tran7389814603</t>
-  </si>
-  <si>
-    <t>transaction17389814603</t>
-  </si>
-  <si>
-    <t>1551173680</t>
-  </si>
-  <si>
-    <t>3337404344</t>
-  </si>
-  <si>
-    <t>02.09 PM</t>
-  </si>
-  <si>
-    <t>tran6856383067</t>
-  </si>
-  <si>
-    <t>transaction16856383067</t>
-  </si>
-  <si>
-    <t>2127837201</t>
-  </si>
-  <si>
-    <t>8502634770</t>
-  </si>
-  <si>
-    <t>02.37 PM</t>
-  </si>
-  <si>
-    <t>tran3562013618</t>
-  </si>
-  <si>
-    <t>transaction13562013618</t>
-  </si>
-  <si>
-    <t>8137609279</t>
-  </si>
-  <si>
-    <t>8101033600</t>
-  </si>
-  <si>
-    <t>10.42 AM</t>
-  </si>
-  <si>
-    <t>tran4033254156</t>
-  </si>
-  <si>
-    <t>transaction14033254156</t>
-  </si>
-  <si>
-    <t>9010260475</t>
-  </si>
-  <si>
-    <t>3233928476</t>
-  </si>
-  <si>
-    <t>11.27 AM</t>
-  </si>
-  <si>
-    <t>tran2434301738</t>
-  </si>
-  <si>
-    <t>transaction12434301738</t>
-  </si>
-  <si>
-    <t>8324501356</t>
-  </si>
-  <si>
-    <t>3103095678</t>
-  </si>
-  <si>
-    <t>11.43 AM</t>
-  </si>
-  <si>
-    <t>tran2382787480</t>
-  </si>
-  <si>
-    <t>transaction12382787480</t>
-  </si>
-  <si>
-    <t>5604791330</t>
-  </si>
-  <si>
-    <t>6604400799</t>
-  </si>
-  <si>
-    <t>11.04 AM</t>
-  </si>
-  <si>
-    <t>tran9373311504</t>
-  </si>
-  <si>
-    <t>transaction19373311504</t>
-  </si>
-  <si>
-    <t>2159935254</t>
-  </si>
-  <si>
-    <t>2881138817</t>
-  </si>
-  <si>
-    <t>10.34 AM</t>
-  </si>
-  <si>
-    <t>tran4721508959</t>
-  </si>
-  <si>
-    <t>transaction14721508959</t>
-  </si>
-  <si>
-    <t>1415468306</t>
-  </si>
-  <si>
-    <t>6823181159</t>
-  </si>
-  <si>
-    <t>11.33 AM</t>
-  </si>
-  <si>
-    <t>tran8003571414</t>
-  </si>
-  <si>
-    <t>transaction18003571414</t>
-  </si>
-  <si>
-    <t>7994782914</t>
-  </si>
-  <si>
-    <t>7283057670</t>
-  </si>
-  <si>
-    <t>10.14 AM</t>
+    <t>transaction1993996c3151</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -2901,100 +2378,100 @@
   <dimension ref="A1:CS3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="18.296875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="13.296875" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="20.09765625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="20.796875" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="17.3984375" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="7.59765625" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="14.69921875" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="11.8984375" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="6.796875" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="13.69921875" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="19.3984375" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="12.296875" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="16.59765625" collapsed="true"/>
-    <col min="14" max="15" bestFit="true" customWidth="true" width="17.8984375" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="12.3984375" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" width="18.19921875" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="17.3984375" collapsed="true"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" width="17.796875" collapsed="true"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" width="9.796875" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" width="13.19921875" collapsed="true"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" width="12.3984375" collapsed="true"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" width="12.5" collapsed="true"/>
-    <col min="24" max="24" bestFit="true" customWidth="true" width="10.19921875" collapsed="true"/>
-    <col min="25" max="25" bestFit="true" customWidth="true" width="7.5" collapsed="true"/>
-    <col min="26" max="26" bestFit="true" customWidth="true" width="16.69921875" collapsed="true"/>
-    <col min="27" max="27" bestFit="true" customWidth="true" width="18.3984375" collapsed="true"/>
-    <col min="28" max="28" bestFit="true" customWidth="true" width="15.09765625" collapsed="true"/>
-    <col min="29" max="29" bestFit="true" customWidth="true" width="15.59765625" collapsed="true"/>
-    <col min="30" max="30" bestFit="true" customWidth="true" width="9.59765625" collapsed="true"/>
-    <col min="31" max="31" bestFit="true" customWidth="true" width="11.59765625" collapsed="true"/>
-    <col min="32" max="32" bestFit="true" customWidth="true" width="11.69921875" collapsed="true"/>
-    <col min="33" max="33" bestFit="true" customWidth="true" width="18.296875" collapsed="true"/>
-    <col min="34" max="34" bestFit="true" customWidth="true" width="15.09765625" collapsed="true"/>
-    <col min="35" max="35" bestFit="true" customWidth="true" width="16.8984375" collapsed="true"/>
-    <col min="36" max="39" bestFit="true" customWidth="true" width="21.5" collapsed="true"/>
-    <col min="40" max="40" bestFit="true" customWidth="true" width="30.69921875" collapsed="true"/>
-    <col min="41" max="41" bestFit="true" customWidth="true" width="17.69921875" collapsed="true"/>
-    <col min="42" max="42" bestFit="true" customWidth="true" width="20.0" collapsed="true"/>
-    <col min="43" max="43" bestFit="true" customWidth="true" width="18.69921875" collapsed="true"/>
-    <col min="44" max="44" bestFit="true" customWidth="true" width="24.59765625" collapsed="true"/>
-    <col min="45" max="45" bestFit="true" customWidth="true" width="11.8984375" collapsed="true"/>
-    <col min="46" max="46" bestFit="true" customWidth="true" width="25.09765625" collapsed="true"/>
-    <col min="47" max="47" bestFit="true" customWidth="true" width="25.59765625" collapsed="true"/>
-    <col min="48" max="48" bestFit="true" customWidth="true" width="19.69921875" collapsed="true"/>
-    <col min="49" max="49" bestFit="true" customWidth="true" width="14.19921875" collapsed="true"/>
-    <col min="50" max="50" bestFit="true" customWidth="true" width="15.09765625" collapsed="true"/>
-    <col min="51" max="51" bestFit="true" customWidth="true" width="26.796875" collapsed="true"/>
-    <col min="52" max="52" bestFit="true" customWidth="true" width="28.796875" collapsed="true"/>
-    <col min="53" max="53" bestFit="true" customWidth="true" width="26.796875" collapsed="true"/>
-    <col min="54" max="54" bestFit="true" customWidth="true" width="28.796875" collapsed="true"/>
-    <col min="55" max="55" bestFit="true" customWidth="true" width="26.796875" collapsed="true"/>
-    <col min="56" max="56" bestFit="true" customWidth="true" width="28.796875" collapsed="true"/>
-    <col min="57" max="57" bestFit="true" customWidth="true" width="26.796875" collapsed="true"/>
-    <col min="58" max="58" bestFit="true" customWidth="true" width="28.796875" collapsed="true"/>
-    <col min="59" max="59" bestFit="true" customWidth="true" width="26.796875" collapsed="true"/>
-    <col min="60" max="60" bestFit="true" customWidth="true" width="28.796875" collapsed="true"/>
-    <col min="61" max="61" bestFit="true" customWidth="true" width="26.796875" collapsed="true"/>
-    <col min="62" max="62" bestFit="true" customWidth="true" width="28.796875" collapsed="true"/>
-    <col min="63" max="63" bestFit="true" customWidth="true" width="18.8984375" collapsed="true"/>
-    <col min="64" max="65" bestFit="true" customWidth="true" width="21.796875" collapsed="true"/>
-    <col min="66" max="66" bestFit="true" customWidth="true" width="20.69921875" collapsed="true"/>
-    <col min="67" max="67" bestFit="true" customWidth="true" width="20.0" collapsed="true"/>
-    <col min="68" max="69" bestFit="true" customWidth="true" width="22.8984375" collapsed="true"/>
-    <col min="70" max="70" bestFit="true" customWidth="true" width="21.8984375" collapsed="true"/>
-    <col min="71" max="71" bestFit="true" customWidth="true" width="16.8984375" collapsed="true"/>
-    <col min="72" max="72" bestFit="true" customWidth="true" width="13.3984375" collapsed="true"/>
-    <col min="73" max="73" bestFit="true" customWidth="true" width="13.296875" collapsed="true"/>
-    <col min="74" max="74" bestFit="true" customWidth="true" width="25.296875" collapsed="true"/>
-    <col min="75" max="75" bestFit="true" customWidth="true" width="9.796875" collapsed="true"/>
-    <col min="76" max="76" bestFit="true" customWidth="true" width="13.3984375" collapsed="true"/>
-    <col min="77" max="77" bestFit="true" customWidth="true" width="15.296875" collapsed="true"/>
-    <col min="78" max="79" bestFit="true" customWidth="true" width="21.5" collapsed="true"/>
-    <col min="80" max="80" bestFit="true" customWidth="true" width="26.0" collapsed="true"/>
-    <col min="81" max="81" bestFit="true" customWidth="true" width="7.09765625" collapsed="true"/>
-    <col min="82" max="82" bestFit="true" customWidth="true" width="5.09765625" collapsed="true"/>
-    <col min="83" max="83" bestFit="true" customWidth="true" width="19.0" collapsed="true"/>
-    <col min="84" max="84" bestFit="true" customWidth="true" width="7.19921875" collapsed="true"/>
-    <col min="85" max="85" bestFit="true" customWidth="true" width="15.796875" collapsed="true"/>
-    <col min="86" max="86" bestFit="true" customWidth="true" width="17.09765625" collapsed="true"/>
-    <col min="87" max="87" bestFit="true" customWidth="true" width="20.0" collapsed="true"/>
-    <col min="88" max="89" bestFit="true" customWidth="true" width="21.8984375" collapsed="true"/>
-    <col min="90" max="90" bestFit="true" customWidth="true" width="17.5" collapsed="true"/>
-    <col min="91" max="91" bestFit="true" customWidth="true" width="19.296875" collapsed="true"/>
-    <col min="92" max="92" bestFit="true" customWidth="true" width="21.19921875" collapsed="true"/>
-    <col min="93" max="93" bestFit="true" customWidth="true" width="16.8984375" collapsed="true"/>
-    <col min="94" max="94" bestFit="true" customWidth="true" width="17.19921875" collapsed="true"/>
-    <col min="95" max="95" bestFit="true" customWidth="true" width="4.09765625" collapsed="true"/>
-    <col min="96" max="96" bestFit="true" customWidth="true" width="4.3984375" collapsed="true"/>
-    <col min="97" max="97" bestFit="true" customWidth="true" width="5.796875" collapsed="true"/>
+    <col min="1" max="1" width="18.296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="13.296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="20.09765625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="20.796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="17.3984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="7.59765625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="14.69921875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="11.8984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="6.796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="13.69921875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="19.3984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="12.296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="16.59765625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="15" width="17.8984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="12.3984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="18.19921875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="17.3984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="17.796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="9.796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="13.19921875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="12.3984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="12.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="10.19921875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="7.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="16.69921875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="18.3984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="15.09765625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="15.59765625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="9.59765625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="11.59765625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="32" max="32" width="11.69921875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="33" max="33" width="18.296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="34" max="34" width="15.09765625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="35" max="35" width="16.8984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="36" max="39" width="21.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="40" max="40" width="30.69921875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="41" max="41" width="17.69921875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="42" max="42" width="20" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="43" max="43" width="18.69921875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="44" max="44" width="24.59765625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="45" max="45" width="11.8984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="46" max="46" width="25.09765625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="47" max="47" width="25.59765625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="48" max="48" width="19.69921875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="49" max="49" width="14.19921875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="50" max="50" width="15.09765625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="51" max="51" width="26.796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="52" max="52" width="28.796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="53" max="53" width="26.796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="54" max="54" width="28.796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="55" max="55" width="26.796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="56" max="56" width="28.796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="57" max="57" width="26.796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="58" max="58" width="28.796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="59" max="59" width="26.796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="60" max="60" width="28.796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="61" max="61" width="26.796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="62" max="62" width="28.796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="63" max="63" width="18.8984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="64" max="65" width="21.796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="66" max="66" width="20.69921875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="67" max="67" width="20" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="68" max="69" width="22.8984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="70" max="70" width="21.8984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="71" max="71" width="16.8984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="72" max="72" width="13.3984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="73" max="73" width="13.296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="74" max="74" width="25.296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="75" max="75" width="9.796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="76" max="76" width="13.3984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="77" max="77" width="15.296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="78" max="79" width="21.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="80" max="80" width="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="81" max="81" width="7.09765625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="82" max="82" width="5.09765625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="83" max="83" width="19" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="84" max="84" width="7.19921875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="85" max="85" width="15.796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="86" max="86" width="17.09765625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="87" max="87" width="20" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="88" max="89" width="21.8984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="90" max="90" width="17.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="91" max="91" width="19.296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="92" max="92" width="21.19921875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="93" max="93" width="16.8984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="94" max="94" width="17.19921875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="95" max="95" width="4.09765625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="96" max="96" width="4.3984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="97" max="97" width="5.796875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:97" x14ac:dyDescent="0.3">
@@ -3292,10 +2769,10 @@
     </row>
     <row r="2" spans="1:97" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>824</v>
+        <v>653</v>
       </c>
       <c r="B2" t="s">
-        <v>826</v>
+        <v>650</v>
       </c>
       <c r="C2" t="s">
         <v>488</v>
@@ -3355,7 +2832,7 @@
         <v>109</v>
       </c>
       <c r="V2" t="s">
-        <v>828</v>
+        <v>652</v>
       </c>
       <c r="W2" s="1" t="s">
         <v>103</v>
@@ -3553,10 +3030,10 @@
     </row>
     <row r="3" spans="1:97" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>825</v>
+        <v>654</v>
       </c>
       <c r="B3" t="s">
-        <v>827</v>
+        <v>651</v>
       </c>
       <c r="C3" t="s">
         <v>488</v>
@@ -3577,7 +3054,7 @@
         <v>109</v>
       </c>
       <c r="V3" t="s">
-        <v>828</v>
+        <v>652</v>
       </c>
       <c r="W3" s="1" t="s">
         <v>103</v>
@@ -3654,209 +3131,209 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="30.69921875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="36.0" collapsed="true"/>
-    <col min="3" max="5" bestFit="true" customWidth="true" width="30.69921875" collapsed="true"/>
-    <col min="6" max="7" bestFit="true" customWidth="true" width="21.5" collapsed="true"/>
-    <col min="8" max="9" bestFit="true" customWidth="true" width="21.8984375" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="25.09765625" collapsed="true"/>
-    <col min="11" max="13" bestFit="true" customWidth="true" width="25.59765625" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="30.69921875" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="26.796875" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="28.796875" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" width="30.69921875" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="28.796875" collapsed="true"/>
-    <col min="19" max="20" bestFit="true" customWidth="true" width="30.69921875" collapsed="true"/>
-    <col min="21" max="26" bestFit="true" customWidth="true" width="28.796875" collapsed="true"/>
-    <col min="27" max="29" bestFit="true" customWidth="true" width="30.69921875" collapsed="true"/>
-    <col min="30" max="40" bestFit="true" customWidth="true" width="28.796875" collapsed="true"/>
-    <col min="41" max="41" bestFit="true" customWidth="true" width="18.8984375" collapsed="true"/>
-    <col min="42" max="43" bestFit="true" customWidth="true" width="21.796875" collapsed="true"/>
-    <col min="44" max="44" bestFit="true" customWidth="true" width="20.69921875" collapsed="true"/>
-    <col min="45" max="45" bestFit="true" customWidth="true" width="20.0" collapsed="true"/>
-    <col min="46" max="47" bestFit="true" customWidth="true" width="22.8984375" collapsed="true"/>
-    <col min="48" max="48" bestFit="true" customWidth="true" width="21.8984375" collapsed="true"/>
-    <col min="49" max="49" bestFit="true" customWidth="true" width="16.8984375" collapsed="true"/>
-    <col min="50" max="50" bestFit="true" customWidth="true" width="13.3984375" collapsed="true"/>
-    <col min="51" max="51" bestFit="true" customWidth="true" width="5.0" collapsed="true"/>
-    <col min="52" max="52" bestFit="true" customWidth="true" width="4.3984375" collapsed="true"/>
-    <col min="53" max="53" bestFit="true" customWidth="true" width="4.296875" collapsed="true"/>
-    <col min="54" max="54" bestFit="true" customWidth="true" width="4.3984375" collapsed="true"/>
-    <col min="55" max="55" bestFit="true" customWidth="true" width="4.296875" collapsed="true"/>
-    <col min="56" max="56" bestFit="true" customWidth="true" width="4.8984375" collapsed="true"/>
-    <col min="57" max="57" bestFit="true" customWidth="true" width="4.796875" collapsed="true"/>
-    <col min="58" max="58" bestFit="true" customWidth="true" width="3.796875" collapsed="true"/>
-    <col min="59" max="59" bestFit="true" customWidth="true" width="4.3984375" collapsed="true"/>
-    <col min="60" max="60" bestFit="true" customWidth="true" width="4.09765625" collapsed="true"/>
-    <col min="61" max="61" bestFit="true" customWidth="true" width="4.3984375" collapsed="true"/>
-    <col min="62" max="62" bestFit="true" customWidth="true" width="4.5" collapsed="true"/>
-    <col min="63" max="63" bestFit="true" customWidth="true" width="4.69921875" collapsed="true"/>
-    <col min="64" max="64" bestFit="true" customWidth="true" width="4.5" collapsed="true"/>
-    <col min="65" max="65" bestFit="true" customWidth="true" width="4.69921875" collapsed="true"/>
-    <col min="66" max="66" bestFit="true" customWidth="true" width="4.09765625" collapsed="true"/>
-    <col min="67" max="67" bestFit="true" customWidth="true" width="4.296875" collapsed="true"/>
-    <col min="68" max="68" bestFit="true" customWidth="true" width="4.19921875" collapsed="true"/>
-    <col min="69" max="69" bestFit="true" customWidth="true" width="4.296875" collapsed="true"/>
-    <col min="70" max="70" bestFit="true" customWidth="true" width="4.5" collapsed="true"/>
-    <col min="71" max="71" bestFit="true" customWidth="true" width="4.3984375" collapsed="true"/>
-    <col min="72" max="72" bestFit="true" customWidth="true" width="5.09765625" collapsed="true"/>
-    <col min="73" max="74" bestFit="true" customWidth="true" width="4.296875" collapsed="true"/>
-    <col min="75" max="75" bestFit="true" customWidth="true" width="4.796875" collapsed="true"/>
-    <col min="76" max="76" bestFit="true" customWidth="true" width="4.8984375" collapsed="true"/>
-    <col min="77" max="77" bestFit="true" customWidth="true" width="4.796875" collapsed="true"/>
-    <col min="78" max="78" bestFit="true" customWidth="true" width="4.8984375" collapsed="true"/>
-    <col min="79" max="80" bestFit="true" customWidth="true" width="4.796875" collapsed="true"/>
-    <col min="81" max="81" bestFit="true" customWidth="true" width="4.0" collapsed="true"/>
-    <col min="82" max="82" bestFit="true" customWidth="true" width="4.8984375" collapsed="true"/>
-    <col min="83" max="83" bestFit="true" customWidth="true" width="4.5" collapsed="true"/>
-    <col min="84" max="84" bestFit="true" customWidth="true" width="4.8984375" collapsed="true"/>
-    <col min="85" max="85" bestFit="true" customWidth="true" width="4.5" collapsed="true"/>
-    <col min="86" max="86" bestFit="true" customWidth="true" width="4.296875" collapsed="true"/>
-    <col min="87" max="87" bestFit="true" customWidth="true" width="4.09765625" collapsed="true"/>
-    <col min="88" max="88" bestFit="true" customWidth="true" width="4.3984375" collapsed="true"/>
-    <col min="89" max="91" bestFit="true" customWidth="true" width="4.796875" collapsed="true"/>
-    <col min="92" max="92" bestFit="true" customWidth="true" width="5.296875" collapsed="true"/>
-    <col min="93" max="93" bestFit="true" customWidth="true" width="4.8984375" collapsed="true"/>
-    <col min="94" max="94" bestFit="true" customWidth="true" width="5.296875" collapsed="true"/>
-    <col min="95" max="95" bestFit="true" customWidth="true" width="4.8984375" collapsed="true"/>
-    <col min="96" max="96" bestFit="true" customWidth="true" width="5.0" collapsed="true"/>
-    <col min="97" max="97" bestFit="true" customWidth="true" width="4.8984375" collapsed="true"/>
-    <col min="98" max="98" bestFit="true" customWidth="true" width="4.796875" collapsed="true"/>
-    <col min="99" max="99" bestFit="true" customWidth="true" width="5.19921875" collapsed="true"/>
-    <col min="100" max="100" bestFit="true" customWidth="true" width="4.796875" collapsed="true"/>
-    <col min="101" max="101" bestFit="true" customWidth="true" width="5.19921875" collapsed="true"/>
-    <col min="102" max="102" bestFit="true" customWidth="true" width="4.796875" collapsed="true"/>
-    <col min="103" max="103" bestFit="true" customWidth="true" width="4.8984375" collapsed="true"/>
-    <col min="104" max="104" bestFit="true" customWidth="true" width="4.296875" collapsed="true"/>
-    <col min="105" max="105" bestFit="true" customWidth="true" width="4.796875" collapsed="true"/>
-    <col min="106" max="107" bestFit="true" customWidth="true" width="4.19921875" collapsed="true"/>
-    <col min="108" max="108" bestFit="true" customWidth="true" width="4.09765625" collapsed="true"/>
-    <col min="109" max="109" bestFit="true" customWidth="true" width="4.59765625" collapsed="true"/>
-    <col min="110" max="110" bestFit="true" customWidth="true" width="4.3984375" collapsed="true"/>
-    <col min="111" max="111" bestFit="true" customWidth="true" width="4.59765625" collapsed="true"/>
-    <col min="112" max="114" bestFit="true" customWidth="true" width="4.69921875" collapsed="true"/>
-    <col min="115" max="116" bestFit="true" customWidth="true" width="4.19921875" collapsed="true"/>
-    <col min="117" max="117" bestFit="true" customWidth="true" width="4.0" collapsed="true"/>
-    <col min="118" max="119" bestFit="true" customWidth="true" width="4.19921875" collapsed="true"/>
-    <col min="120" max="121" bestFit="true" customWidth="true" width="4.5" collapsed="true"/>
-    <col min="122" max="122" bestFit="true" customWidth="true" width="4.59765625" collapsed="true"/>
-    <col min="123" max="123" bestFit="true" customWidth="true" width="4.296875" collapsed="true"/>
-    <col min="124" max="124" bestFit="true" customWidth="true" width="4.09765625" collapsed="true"/>
-    <col min="125" max="125" bestFit="true" customWidth="true" width="5.296875" collapsed="true"/>
-    <col min="126" max="126" bestFit="true" customWidth="true" width="4.3984375" collapsed="true"/>
-    <col min="127" max="127" bestFit="true" customWidth="true" width="5.296875" collapsed="true"/>
-    <col min="128" max="128" bestFit="true" customWidth="true" width="4.8984375" collapsed="true"/>
-    <col min="129" max="129" bestFit="true" customWidth="true" width="4.59765625" collapsed="true"/>
-    <col min="130" max="130" bestFit="true" customWidth="true" width="4.5" collapsed="true"/>
-    <col min="131" max="131" bestFit="true" customWidth="true" width="4.796875" collapsed="true"/>
-    <col min="132" max="133" bestFit="true" customWidth="true" width="4.5" collapsed="true"/>
-    <col min="134" max="134" bestFit="true" customWidth="true" width="4.3984375" collapsed="true"/>
-    <col min="135" max="135" bestFit="true" customWidth="true" width="4.59765625" collapsed="true"/>
-    <col min="136" max="136" bestFit="true" customWidth="true" width="4.3984375" collapsed="true"/>
-    <col min="137" max="137" bestFit="true" customWidth="true" width="4.59765625" collapsed="true"/>
-    <col min="138" max="138" bestFit="true" customWidth="true" width="4.796875" collapsed="true"/>
-    <col min="139" max="141" bestFit="true" customWidth="true" width="4.8984375" collapsed="true"/>
-    <col min="142" max="142" bestFit="true" customWidth="true" width="4.59765625" collapsed="true"/>
-    <col min="143" max="143" bestFit="true" customWidth="true" width="4.19921875" collapsed="true"/>
-    <col min="144" max="144" bestFit="true" customWidth="true" width="4.59765625" collapsed="true"/>
-    <col min="145" max="145" bestFit="true" customWidth="true" width="4.3984375" collapsed="true"/>
-    <col min="146" max="146" bestFit="true" customWidth="true" width="5.0" collapsed="true"/>
-    <col min="147" max="147" bestFit="true" customWidth="true" width="4.3984375" collapsed="true"/>
-    <col min="148" max="148" bestFit="true" customWidth="true" width="5.0" collapsed="true"/>
-    <col min="149" max="149" bestFit="true" customWidth="true" width="4.3984375" collapsed="true"/>
-    <col min="150" max="150" bestFit="true" customWidth="true" width="4.796875" collapsed="true"/>
-    <col min="151" max="151" bestFit="true" customWidth="true" width="4.296875" collapsed="true"/>
-    <col min="152" max="152" bestFit="true" customWidth="true" width="4.796875" collapsed="true"/>
-    <col min="153" max="153" bestFit="true" customWidth="true" width="4.296875" collapsed="true"/>
-    <col min="154" max="154" bestFit="true" customWidth="true" width="4.796875" collapsed="true"/>
-    <col min="155" max="156" bestFit="true" customWidth="true" width="4.296875" collapsed="true"/>
-    <col min="157" max="157" bestFit="true" customWidth="true" width="4.3984375" collapsed="true"/>
-    <col min="158" max="158" bestFit="true" customWidth="true" width="4.09765625" collapsed="true"/>
-    <col min="159" max="159" bestFit="true" customWidth="true" width="3.796875" collapsed="true"/>
-    <col min="160" max="160" bestFit="true" customWidth="true" width="4.19921875" collapsed="true"/>
-    <col min="161" max="161" bestFit="true" customWidth="true" width="4.8984375" collapsed="true"/>
-    <col min="162" max="162" bestFit="true" customWidth="true" width="3.796875" collapsed="true"/>
-    <col min="163" max="163" bestFit="true" customWidth="true" width="4.8984375" collapsed="true"/>
-    <col min="164" max="165" bestFit="true" customWidth="true" width="5.0" collapsed="true"/>
-    <col min="166" max="166" bestFit="true" customWidth="true" width="5.3984375" collapsed="true"/>
-    <col min="167" max="167" bestFit="true" customWidth="true" width="5.0" collapsed="true"/>
-    <col min="168" max="168" bestFit="true" customWidth="true" width="5.3984375" collapsed="true"/>
-    <col min="169" max="169" bestFit="true" customWidth="true" width="4.69921875" collapsed="true"/>
-    <col min="170" max="170" bestFit="true" customWidth="true" width="4.59765625" collapsed="true"/>
-    <col min="171" max="171" bestFit="true" customWidth="true" width="4.296875" collapsed="true"/>
-    <col min="172" max="172" bestFit="true" customWidth="true" width="5.0" collapsed="true"/>
-    <col min="173" max="173" bestFit="true" customWidth="true" width="4.5" collapsed="true"/>
-    <col min="174" max="174" bestFit="true" customWidth="true" width="5.19921875" collapsed="true"/>
-    <col min="175" max="175" bestFit="true" customWidth="true" width="4.5" collapsed="true"/>
-    <col min="176" max="176" bestFit="true" customWidth="true" width="4.8984375" collapsed="true"/>
-    <col min="177" max="177" bestFit="true" customWidth="true" width="5.0" collapsed="true"/>
-    <col min="178" max="178" bestFit="true" customWidth="true" width="4.69921875" collapsed="true"/>
-    <col min="179" max="179" bestFit="true" customWidth="true" width="4.19921875" collapsed="true"/>
-    <col min="180" max="180" bestFit="true" customWidth="true" width="4.3984375" collapsed="true"/>
-    <col min="181" max="181" bestFit="true" customWidth="true" width="4.19921875" collapsed="true"/>
-    <col min="182" max="182" bestFit="true" customWidth="true" width="4.3984375" collapsed="true"/>
-    <col min="183" max="183" bestFit="true" customWidth="true" width="4.296875" collapsed="true"/>
-    <col min="184" max="184" bestFit="true" customWidth="true" width="5.19921875" collapsed="true"/>
-    <col min="185" max="185" bestFit="true" customWidth="true" width="5.296875" collapsed="true"/>
-    <col min="186" max="186" bestFit="true" customWidth="true" width="4.296875" collapsed="true"/>
-    <col min="187" max="187" bestFit="true" customWidth="true" width="4.19921875" collapsed="true"/>
-    <col min="188" max="188" bestFit="true" customWidth="true" width="4.296875" collapsed="true"/>
-    <col min="189" max="189" bestFit="true" customWidth="true" width="4.09765625" collapsed="true"/>
-    <col min="190" max="190" bestFit="true" customWidth="true" width="4.5" collapsed="true"/>
-    <col min="191" max="191" bestFit="true" customWidth="true" width="5.296875" collapsed="true"/>
-    <col min="192" max="192" bestFit="true" customWidth="true" width="4.5" collapsed="true"/>
-    <col min="193" max="193" bestFit="true" customWidth="true" width="5.296875" collapsed="true"/>
-    <col min="194" max="194" bestFit="true" customWidth="true" width="4.5" collapsed="true"/>
-    <col min="195" max="195" bestFit="true" customWidth="true" width="4.296875" collapsed="true"/>
-    <col min="196" max="196" bestFit="true" customWidth="true" width="3.3984375" collapsed="true"/>
-    <col min="197" max="197" bestFit="true" customWidth="true" width="4.59765625" collapsed="true"/>
-    <col min="198" max="198" bestFit="true" customWidth="true" width="3.796875" collapsed="true"/>
-    <col min="199" max="199" bestFit="true" customWidth="true" width="4.09765625" collapsed="true"/>
-    <col min="200" max="200" bestFit="true" customWidth="true" width="4.3984375" collapsed="true"/>
-    <col min="201" max="201" bestFit="true" customWidth="true" width="2.296875" collapsed="true"/>
-    <col min="202" max="202" bestFit="true" customWidth="true" width="2.3984375" collapsed="true"/>
-    <col min="203" max="203" bestFit="true" customWidth="true" width="2.796875" collapsed="true"/>
-    <col min="204" max="204" bestFit="true" customWidth="true" width="2.59765625" collapsed="true"/>
-    <col min="205" max="205" bestFit="true" customWidth="true" width="3.5" collapsed="true"/>
-    <col min="206" max="207" bestFit="true" customWidth="true" width="3.09765625" collapsed="true"/>
-    <col min="208" max="208" bestFit="true" customWidth="true" width="2.8984375" collapsed="true"/>
-    <col min="209" max="209" bestFit="true" customWidth="true" width="2.69921875" collapsed="true"/>
-    <col min="210" max="210" bestFit="true" customWidth="true" width="2.796875" collapsed="true"/>
-    <col min="211" max="211" bestFit="true" customWidth="true" width="2.8984375" collapsed="true"/>
-    <col min="212" max="213" bestFit="true" customWidth="true" width="2.796875" collapsed="true"/>
-    <col min="214" max="214" bestFit="true" customWidth="true" width="2.69921875" collapsed="true"/>
-    <col min="215" max="215" bestFit="true" customWidth="true" width="3.0" collapsed="true"/>
-    <col min="216" max="216" bestFit="true" customWidth="true" width="3.09765625" collapsed="true"/>
-    <col min="217" max="217" bestFit="true" customWidth="true" width="2.796875" collapsed="true"/>
-    <col min="218" max="218" bestFit="true" customWidth="true" width="3.19921875" collapsed="true"/>
-    <col min="219" max="219" bestFit="true" customWidth="true" width="3.09765625" collapsed="true"/>
-    <col min="220" max="220" bestFit="true" customWidth="true" width="2.5" collapsed="true"/>
-    <col min="221" max="221" bestFit="true" customWidth="true" width="2.8984375" collapsed="true"/>
-    <col min="222" max="222" bestFit="true" customWidth="true" width="2.69921875" collapsed="true"/>
-    <col min="223" max="223" bestFit="true" customWidth="true" width="3.59765625" collapsed="true"/>
-    <col min="224" max="225" bestFit="true" customWidth="true" width="3.19921875" collapsed="true"/>
-    <col min="226" max="226" bestFit="true" customWidth="true" width="3.0" collapsed="true"/>
-    <col min="227" max="227" bestFit="true" customWidth="true" width="2.8984375" collapsed="true"/>
-    <col min="228" max="228" bestFit="true" customWidth="true" width="3.0" collapsed="true"/>
-    <col min="229" max="229" bestFit="true" customWidth="true" width="3.69921875" collapsed="true"/>
-    <col min="230" max="230" bestFit="true" customWidth="true" width="2.796875" collapsed="true"/>
-    <col min="231" max="231" bestFit="true" customWidth="true" width="3.3984375" collapsed="true"/>
-    <col min="232" max="232" bestFit="true" customWidth="true" width="3.5" collapsed="true"/>
-    <col min="233" max="233" bestFit="true" customWidth="true" width="3.8984375" collapsed="true"/>
-    <col min="234" max="234" bestFit="true" customWidth="true" width="3.09765625" collapsed="true"/>
-    <col min="235" max="235" bestFit="true" customWidth="true" width="3.19921875" collapsed="true"/>
-    <col min="236" max="236" bestFit="true" customWidth="true" width="3.09765625" collapsed="true"/>
-    <col min="237" max="237" bestFit="true" customWidth="true" width="3.19921875" collapsed="true"/>
-    <col min="238" max="238" bestFit="true" customWidth="true" width="3.09765625" collapsed="true"/>
-    <col min="239" max="239" bestFit="true" customWidth="true" width="3.0" collapsed="true"/>
-    <col min="240" max="240" bestFit="true" customWidth="true" width="3.296875" collapsed="true"/>
-    <col min="241" max="241" bestFit="true" customWidth="true" width="2.5" collapsed="true"/>
-    <col min="242" max="243" bestFit="true" customWidth="true" width="3.296875" collapsed="true"/>
-    <col min="244" max="245" bestFit="true" customWidth="true" width="3.59765625" collapsed="true"/>
-    <col min="246" max="247" bestFit="true" customWidth="true" width="2.8984375" collapsed="true"/>
-    <col min="248" max="248" bestFit="true" customWidth="true" width="3.0" collapsed="true"/>
-    <col min="249" max="249" bestFit="true" customWidth="true" width="3.5" collapsed="true"/>
-    <col min="250" max="250" bestFit="true" customWidth="true" width="3.59765625" collapsed="true"/>
+    <col min="1" max="1" width="30.69921875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="36" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="5" width="30.69921875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="7" width="21.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="9" width="21.8984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="25.09765625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="13" width="25.59765625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="30.69921875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="26.796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="28.796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="30.69921875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="28.796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="20" width="30.69921875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="26" width="28.796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="29" width="30.69921875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="30" max="40" width="28.796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="41" max="41" width="18.8984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="42" max="43" width="21.796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="44" max="44" width="20.69921875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="45" max="45" width="20" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="46" max="47" width="22.8984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="48" max="48" width="21.8984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="49" max="49" width="16.8984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="50" max="50" width="13.3984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="51" max="51" width="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="52" max="52" width="4.3984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="53" max="53" width="4.296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="54" max="54" width="4.3984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="55" max="55" width="4.296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="56" max="56" width="4.8984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="57" max="57" width="4.796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="58" max="58" width="3.796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="59" max="59" width="4.3984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="60" max="60" width="4.09765625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="61" max="61" width="4.3984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="62" max="62" width="4.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="63" max="63" width="4.69921875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="64" max="64" width="4.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="65" max="65" width="4.69921875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="66" max="66" width="4.09765625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="67" max="67" width="4.296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="68" max="68" width="4.19921875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="69" max="69" width="4.296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="70" max="70" width="4.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="71" max="71" width="4.3984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="72" max="72" width="5.09765625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="73" max="74" width="4.296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="75" max="75" width="4.796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="76" max="76" width="4.8984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="77" max="77" width="4.796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="78" max="78" width="4.8984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="79" max="80" width="4.796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="81" max="81" width="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="82" max="82" width="4.8984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="83" max="83" width="4.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="84" max="84" width="4.8984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="85" max="85" width="4.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="86" max="86" width="4.296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="87" max="87" width="4.09765625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="88" max="88" width="4.3984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="89" max="91" width="4.796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="92" max="92" width="5.296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="93" max="93" width="4.8984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="94" max="94" width="5.296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="95" max="95" width="4.8984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="96" max="96" width="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="97" max="97" width="4.8984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="98" max="98" width="4.796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="99" max="99" width="5.19921875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="100" max="100" width="4.796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="101" max="101" width="5.19921875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="102" max="102" width="4.796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="103" max="103" width="4.8984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="104" max="104" width="4.296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="105" max="105" width="4.796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="106" max="107" width="4.19921875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="108" max="108" width="4.09765625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="109" max="109" width="4.59765625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="110" max="110" width="4.3984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="111" max="111" width="4.59765625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="112" max="114" width="4.69921875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="115" max="116" width="4.19921875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="117" max="117" width="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="118" max="119" width="4.19921875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="120" max="121" width="4.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="122" max="122" width="4.59765625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="123" max="123" width="4.296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="124" max="124" width="4.09765625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="125" max="125" width="5.296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="126" max="126" width="4.3984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="127" max="127" width="5.296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="128" max="128" width="4.8984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="129" max="129" width="4.59765625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="130" max="130" width="4.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="131" max="131" width="4.796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="132" max="133" width="4.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="134" max="134" width="4.3984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="135" max="135" width="4.59765625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="136" max="136" width="4.3984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="137" max="137" width="4.59765625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="138" max="138" width="4.796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="139" max="141" width="4.8984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="142" max="142" width="4.59765625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="143" max="143" width="4.19921875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="144" max="144" width="4.59765625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="145" max="145" width="4.3984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="146" max="146" width="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="147" max="147" width="4.3984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="148" max="148" width="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="149" max="149" width="4.3984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="150" max="150" width="4.796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="151" max="151" width="4.296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="152" max="152" width="4.796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="153" max="153" width="4.296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="154" max="154" width="4.796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="155" max="156" width="4.296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="157" max="157" width="4.3984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="158" max="158" width="4.09765625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="159" max="159" width="3.796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="160" max="160" width="4.19921875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="161" max="161" width="4.8984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="162" max="162" width="3.796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="163" max="163" width="4.8984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="164" max="165" width="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="166" max="166" width="5.3984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="167" max="167" width="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="168" max="168" width="5.3984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="169" max="169" width="4.69921875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="170" max="170" width="4.59765625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="171" max="171" width="4.296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="172" max="172" width="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="173" max="173" width="4.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="174" max="174" width="5.19921875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="175" max="175" width="4.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="176" max="176" width="4.8984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="177" max="177" width="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="178" max="178" width="4.69921875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="179" max="179" width="4.19921875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="180" max="180" width="4.3984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="181" max="181" width="4.19921875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="182" max="182" width="4.3984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="183" max="183" width="4.296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="184" max="184" width="5.19921875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="185" max="185" width="5.296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="186" max="186" width="4.296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="187" max="187" width="4.19921875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="188" max="188" width="4.296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="189" max="189" width="4.09765625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="190" max="190" width="4.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="191" max="191" width="5.296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="192" max="192" width="4.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="193" max="193" width="5.296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="194" max="194" width="4.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="195" max="195" width="4.296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="196" max="196" width="3.3984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="197" max="197" width="4.59765625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="198" max="198" width="3.796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="199" max="199" width="4.09765625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="200" max="200" width="4.3984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="201" max="201" width="2.296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="202" max="202" width="2.3984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="203" max="203" width="2.796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="204" max="204" width="2.59765625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="205" max="205" width="3.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="206" max="207" width="3.09765625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="208" max="208" width="2.8984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="209" max="209" width="2.69921875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="210" max="210" width="2.796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="211" max="211" width="2.8984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="212" max="213" width="2.796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="214" max="214" width="2.69921875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="215" max="215" width="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="216" max="216" width="3.09765625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="217" max="217" width="2.796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="218" max="218" width="3.19921875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="219" max="219" width="3.09765625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="220" max="220" width="2.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="221" max="221" width="2.8984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="222" max="222" width="2.69921875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="223" max="223" width="3.59765625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="224" max="225" width="3.19921875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="226" max="226" width="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="227" max="227" width="2.8984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="228" max="228" width="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="229" max="229" width="3.69921875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="230" max="230" width="2.796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="231" max="231" width="3.3984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="232" max="232" width="3.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="233" max="233" width="3.8984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="234" max="234" width="3.09765625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="235" max="235" width="3.19921875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="236" max="236" width="3.09765625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="237" max="237" width="3.19921875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="238" max="238" width="3.09765625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="239" max="239" width="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="240" max="240" width="3.296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="241" max="241" width="2.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="242" max="243" width="3.296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="244" max="245" width="3.59765625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="246" max="247" width="2.8984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="248" max="248" width="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="249" max="249" width="3.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="250" max="250" width="3.59765625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:50" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Updated TS08 and TS13
</commit_message>
<xml_diff>
--- a/src/main/resources/Bulk_ConventionalTransactions_File.xlsx
+++ b/src/main/resources/Bulk_ConventionalTransactions_File.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr codeName="ThisWorkbook"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\BDD_Framework\30 March\10MayNew\29May-Main\20 june\upp-test-automation\src\main\resources\"/>
     </mc:Choice>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24393" uniqueCount="655">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24405" uniqueCount="665">
   <si>
     <t>transactionName</t>
   </si>
@@ -1986,11 +1986,42 @@
   <si>
     <t>transaction1993996c3151</t>
   </si>
+  <si>
+    <t>tran1146723078</t>
+  </si>
+  <si>
+    <t>transaction11146723078</t>
+  </si>
+  <si>
+    <t>1642080765</t>
+  </si>
+  <si>
+    <t>2103265690</t>
+  </si>
+  <si>
+    <t>10.18 AM</t>
+  </si>
+  <si>
+    <t>tran8966713347</t>
+  </si>
+  <si>
+    <t>transaction18966713347</t>
+  </si>
+  <si>
+    <t>5616027373</t>
+  </si>
+  <si>
+    <t>5113262304</t>
+  </si>
+  <si>
+    <t>01.46 PM</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -2383,95 +2414,95 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="13.296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="20.09765625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="20.796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="17.3984375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="7.59765625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="14.69921875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="11.8984375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="6.796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="13.69921875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="19.3984375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="12.296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="16.59765625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="15" width="17.8984375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="12.3984375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="18.19921875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="17.3984375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="17.796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="9.796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="13.19921875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="12.3984375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="12.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="10.19921875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="7.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="16.69921875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="18.3984375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="15.09765625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="15.59765625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="30" max="30" width="9.59765625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="31" max="31" width="11.59765625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="32" max="32" width="11.69921875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="33" max="33" width="18.296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="34" max="34" width="15.09765625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="35" max="35" width="16.8984375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="36" max="39" width="21.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="40" max="40" width="30.69921875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="41" max="41" width="17.69921875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="42" max="42" width="20" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="43" max="43" width="18.69921875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="44" max="44" width="24.59765625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="45" max="45" width="11.8984375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="46" max="46" width="25.09765625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="47" max="47" width="25.59765625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="48" max="48" width="19.69921875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="49" max="49" width="14.19921875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="50" max="50" width="15.09765625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="51" max="51" width="26.796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="52" max="52" width="28.796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="53" max="53" width="26.796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="54" max="54" width="28.796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="55" max="55" width="26.796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="56" max="56" width="28.796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="57" max="57" width="26.796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="58" max="58" width="28.796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="59" max="59" width="26.796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="60" max="60" width="28.796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="61" max="61" width="26.796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="62" max="62" width="28.796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="63" max="63" width="18.8984375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="64" max="65" width="21.796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="66" max="66" width="20.69921875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="67" max="67" width="20" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="68" max="69" width="22.8984375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="70" max="70" width="21.8984375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="71" max="71" width="16.8984375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="72" max="72" width="13.3984375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="73" max="73" width="13.296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="74" max="74" width="25.296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="75" max="75" width="9.796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="76" max="76" width="13.3984375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="77" max="77" width="15.296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="78" max="79" width="21.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="80" max="80" width="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="81" max="81" width="7.09765625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="82" max="82" width="5.09765625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="83" max="83" width="19" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="84" max="84" width="7.19921875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="85" max="85" width="15.796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="86" max="86" width="17.09765625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="87" max="87" width="20" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="88" max="89" width="21.8984375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="90" max="90" width="17.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="91" max="91" width="19.296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="92" max="92" width="21.19921875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="93" max="93" width="16.8984375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="94" max="94" width="17.19921875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="95" max="95" width="4.09765625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="96" max="96" width="4.3984375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="97" max="97" width="5.796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="18.296875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="13.296875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="20.09765625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="20.796875" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="17.3984375" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="7.59765625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="14.69921875" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="11.8984375" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="6.796875" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="13.69921875" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="19.3984375" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="12.296875" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="16.59765625" collapsed="true"/>
+    <col min="14" max="15" bestFit="true" customWidth="true" width="17.8984375" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="12.3984375" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="18.19921875" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="17.3984375" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" width="17.796875" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" width="9.796875" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" width="13.19921875" collapsed="true"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" width="12.3984375" collapsed="true"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" width="12.5" collapsed="true"/>
+    <col min="24" max="24" bestFit="true" customWidth="true" width="10.19921875" collapsed="true"/>
+    <col min="25" max="25" bestFit="true" customWidth="true" width="7.5" collapsed="true"/>
+    <col min="26" max="26" bestFit="true" customWidth="true" width="16.69921875" collapsed="true"/>
+    <col min="27" max="27" bestFit="true" customWidth="true" width="18.3984375" collapsed="true"/>
+    <col min="28" max="28" bestFit="true" customWidth="true" width="15.09765625" collapsed="true"/>
+    <col min="29" max="29" bestFit="true" customWidth="true" width="15.59765625" collapsed="true"/>
+    <col min="30" max="30" bestFit="true" customWidth="true" width="9.59765625" collapsed="true"/>
+    <col min="31" max="31" bestFit="true" customWidth="true" width="11.59765625" collapsed="true"/>
+    <col min="32" max="32" bestFit="true" customWidth="true" width="11.69921875" collapsed="true"/>
+    <col min="33" max="33" bestFit="true" customWidth="true" width="18.296875" collapsed="true"/>
+    <col min="34" max="34" bestFit="true" customWidth="true" width="15.09765625" collapsed="true"/>
+    <col min="35" max="35" bestFit="true" customWidth="true" width="16.8984375" collapsed="true"/>
+    <col min="36" max="39" bestFit="true" customWidth="true" width="21.5" collapsed="true"/>
+    <col min="40" max="40" bestFit="true" customWidth="true" width="30.69921875" collapsed="true"/>
+    <col min="41" max="41" bestFit="true" customWidth="true" width="17.69921875" collapsed="true"/>
+    <col min="42" max="42" bestFit="true" customWidth="true" width="20.0" collapsed="true"/>
+    <col min="43" max="43" bestFit="true" customWidth="true" width="18.69921875" collapsed="true"/>
+    <col min="44" max="44" bestFit="true" customWidth="true" width="24.59765625" collapsed="true"/>
+    <col min="45" max="45" bestFit="true" customWidth="true" width="11.8984375" collapsed="true"/>
+    <col min="46" max="46" bestFit="true" customWidth="true" width="25.09765625" collapsed="true"/>
+    <col min="47" max="47" bestFit="true" customWidth="true" width="25.59765625" collapsed="true"/>
+    <col min="48" max="48" bestFit="true" customWidth="true" width="19.69921875" collapsed="true"/>
+    <col min="49" max="49" bestFit="true" customWidth="true" width="14.19921875" collapsed="true"/>
+    <col min="50" max="50" bestFit="true" customWidth="true" width="15.09765625" collapsed="true"/>
+    <col min="51" max="51" bestFit="true" customWidth="true" width="26.796875" collapsed="true"/>
+    <col min="52" max="52" bestFit="true" customWidth="true" width="28.796875" collapsed="true"/>
+    <col min="53" max="53" bestFit="true" customWidth="true" width="26.796875" collapsed="true"/>
+    <col min="54" max="54" bestFit="true" customWidth="true" width="28.796875" collapsed="true"/>
+    <col min="55" max="55" bestFit="true" customWidth="true" width="26.796875" collapsed="true"/>
+    <col min="56" max="56" bestFit="true" customWidth="true" width="28.796875" collapsed="true"/>
+    <col min="57" max="57" bestFit="true" customWidth="true" width="26.796875" collapsed="true"/>
+    <col min="58" max="58" bestFit="true" customWidth="true" width="28.796875" collapsed="true"/>
+    <col min="59" max="59" bestFit="true" customWidth="true" width="26.796875" collapsed="true"/>
+    <col min="60" max="60" bestFit="true" customWidth="true" width="28.796875" collapsed="true"/>
+    <col min="61" max="61" bestFit="true" customWidth="true" width="26.796875" collapsed="true"/>
+    <col min="62" max="62" bestFit="true" customWidth="true" width="28.796875" collapsed="true"/>
+    <col min="63" max="63" bestFit="true" customWidth="true" width="18.8984375" collapsed="true"/>
+    <col min="64" max="65" bestFit="true" customWidth="true" width="21.796875" collapsed="true"/>
+    <col min="66" max="66" bestFit="true" customWidth="true" width="20.69921875" collapsed="true"/>
+    <col min="67" max="67" bestFit="true" customWidth="true" width="20.0" collapsed="true"/>
+    <col min="68" max="69" bestFit="true" customWidth="true" width="22.8984375" collapsed="true"/>
+    <col min="70" max="70" bestFit="true" customWidth="true" width="21.8984375" collapsed="true"/>
+    <col min="71" max="71" bestFit="true" customWidth="true" width="16.8984375" collapsed="true"/>
+    <col min="72" max="72" bestFit="true" customWidth="true" width="13.3984375" collapsed="true"/>
+    <col min="73" max="73" bestFit="true" customWidth="true" width="13.296875" collapsed="true"/>
+    <col min="74" max="74" bestFit="true" customWidth="true" width="25.296875" collapsed="true"/>
+    <col min="75" max="75" bestFit="true" customWidth="true" width="9.796875" collapsed="true"/>
+    <col min="76" max="76" bestFit="true" customWidth="true" width="13.3984375" collapsed="true"/>
+    <col min="77" max="77" bestFit="true" customWidth="true" width="15.296875" collapsed="true"/>
+    <col min="78" max="79" bestFit="true" customWidth="true" width="21.5" collapsed="true"/>
+    <col min="80" max="80" bestFit="true" customWidth="true" width="26.0" collapsed="true"/>
+    <col min="81" max="81" bestFit="true" customWidth="true" width="7.09765625" collapsed="true"/>
+    <col min="82" max="82" bestFit="true" customWidth="true" width="5.09765625" collapsed="true"/>
+    <col min="83" max="83" bestFit="true" customWidth="true" width="19.0" collapsed="true"/>
+    <col min="84" max="84" bestFit="true" customWidth="true" width="7.19921875" collapsed="true"/>
+    <col min="85" max="85" bestFit="true" customWidth="true" width="15.796875" collapsed="true"/>
+    <col min="86" max="86" bestFit="true" customWidth="true" width="17.09765625" collapsed="true"/>
+    <col min="87" max="87" bestFit="true" customWidth="true" width="20.0" collapsed="true"/>
+    <col min="88" max="89" bestFit="true" customWidth="true" width="21.8984375" collapsed="true"/>
+    <col min="90" max="90" bestFit="true" customWidth="true" width="17.5" collapsed="true"/>
+    <col min="91" max="91" bestFit="true" customWidth="true" width="19.296875" collapsed="true"/>
+    <col min="92" max="92" bestFit="true" customWidth="true" width="21.19921875" collapsed="true"/>
+    <col min="93" max="93" bestFit="true" customWidth="true" width="16.8984375" collapsed="true"/>
+    <col min="94" max="94" bestFit="true" customWidth="true" width="17.19921875" collapsed="true"/>
+    <col min="95" max="95" bestFit="true" customWidth="true" width="4.09765625" collapsed="true"/>
+    <col min="96" max="96" bestFit="true" customWidth="true" width="4.3984375" collapsed="true"/>
+    <col min="97" max="97" bestFit="true" customWidth="true" width="5.796875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:97" x14ac:dyDescent="0.3">
@@ -2769,10 +2800,10 @@
     </row>
     <row r="2" spans="1:97" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>653</v>
+        <v>660</v>
       </c>
       <c r="B2" t="s">
-        <v>650</v>
+        <v>662</v>
       </c>
       <c r="C2" t="s">
         <v>488</v>
@@ -2832,7 +2863,7 @@
         <v>109</v>
       </c>
       <c r="V2" t="s">
-        <v>652</v>
+        <v>664</v>
       </c>
       <c r="W2" s="1" t="s">
         <v>103</v>
@@ -3030,10 +3061,10 @@
     </row>
     <row r="3" spans="1:97" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>654</v>
+        <v>661</v>
       </c>
       <c r="B3" t="s">
-        <v>651</v>
+        <v>663</v>
       </c>
       <c r="C3" t="s">
         <v>488</v>
@@ -3054,7 +3085,7 @@
         <v>109</v>
       </c>
       <c r="V3" t="s">
-        <v>652</v>
+        <v>664</v>
       </c>
       <c r="W3" s="1" t="s">
         <v>103</v>
@@ -3131,209 +3162,209 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="30.69921875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="36" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="5" width="30.69921875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="7" width="21.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="9" width="21.8984375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="25.09765625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="13" width="25.59765625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="30.69921875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="26.796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="28.796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="30.69921875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="28.796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="20" width="30.69921875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="26" width="28.796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="27" max="29" width="30.69921875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="30" max="40" width="28.796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="41" max="41" width="18.8984375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="42" max="43" width="21.796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="44" max="44" width="20.69921875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="45" max="45" width="20" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="46" max="47" width="22.8984375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="48" max="48" width="21.8984375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="49" max="49" width="16.8984375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="50" max="50" width="13.3984375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="51" max="51" width="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="52" max="52" width="4.3984375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="53" max="53" width="4.296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="54" max="54" width="4.3984375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="55" max="55" width="4.296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="56" max="56" width="4.8984375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="57" max="57" width="4.796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="58" max="58" width="3.796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="59" max="59" width="4.3984375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="60" max="60" width="4.09765625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="61" max="61" width="4.3984375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="62" max="62" width="4.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="63" max="63" width="4.69921875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="64" max="64" width="4.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="65" max="65" width="4.69921875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="66" max="66" width="4.09765625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="67" max="67" width="4.296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="68" max="68" width="4.19921875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="69" max="69" width="4.296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="70" max="70" width="4.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="71" max="71" width="4.3984375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="72" max="72" width="5.09765625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="73" max="74" width="4.296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="75" max="75" width="4.796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="76" max="76" width="4.8984375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="77" max="77" width="4.796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="78" max="78" width="4.8984375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="79" max="80" width="4.796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="81" max="81" width="4" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="82" max="82" width="4.8984375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="83" max="83" width="4.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="84" max="84" width="4.8984375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="85" max="85" width="4.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="86" max="86" width="4.296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="87" max="87" width="4.09765625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="88" max="88" width="4.3984375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="89" max="91" width="4.796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="92" max="92" width="5.296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="93" max="93" width="4.8984375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="94" max="94" width="5.296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="95" max="95" width="4.8984375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="96" max="96" width="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="97" max="97" width="4.8984375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="98" max="98" width="4.796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="99" max="99" width="5.19921875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="100" max="100" width="4.796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="101" max="101" width="5.19921875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="102" max="102" width="4.796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="103" max="103" width="4.8984375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="104" max="104" width="4.296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="105" max="105" width="4.796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="106" max="107" width="4.19921875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="108" max="108" width="4.09765625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="109" max="109" width="4.59765625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="110" max="110" width="4.3984375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="111" max="111" width="4.59765625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="112" max="114" width="4.69921875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="115" max="116" width="4.19921875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="117" max="117" width="4" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="118" max="119" width="4.19921875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="120" max="121" width="4.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="122" max="122" width="4.59765625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="123" max="123" width="4.296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="124" max="124" width="4.09765625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="125" max="125" width="5.296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="126" max="126" width="4.3984375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="127" max="127" width="5.296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="128" max="128" width="4.8984375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="129" max="129" width="4.59765625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="130" max="130" width="4.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="131" max="131" width="4.796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="132" max="133" width="4.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="134" max="134" width="4.3984375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="135" max="135" width="4.59765625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="136" max="136" width="4.3984375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="137" max="137" width="4.59765625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="138" max="138" width="4.796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="139" max="141" width="4.8984375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="142" max="142" width="4.59765625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="143" max="143" width="4.19921875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="144" max="144" width="4.59765625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="145" max="145" width="4.3984375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="146" max="146" width="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="147" max="147" width="4.3984375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="148" max="148" width="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="149" max="149" width="4.3984375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="150" max="150" width="4.796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="151" max="151" width="4.296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="152" max="152" width="4.796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="153" max="153" width="4.296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="154" max="154" width="4.796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="155" max="156" width="4.296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="157" max="157" width="4.3984375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="158" max="158" width="4.09765625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="159" max="159" width="3.796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="160" max="160" width="4.19921875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="161" max="161" width="4.8984375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="162" max="162" width="3.796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="163" max="163" width="4.8984375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="164" max="165" width="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="166" max="166" width="5.3984375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="167" max="167" width="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="168" max="168" width="5.3984375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="169" max="169" width="4.69921875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="170" max="170" width="4.59765625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="171" max="171" width="4.296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="172" max="172" width="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="173" max="173" width="4.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="174" max="174" width="5.19921875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="175" max="175" width="4.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="176" max="176" width="4.8984375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="177" max="177" width="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="178" max="178" width="4.69921875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="179" max="179" width="4.19921875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="180" max="180" width="4.3984375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="181" max="181" width="4.19921875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="182" max="182" width="4.3984375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="183" max="183" width="4.296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="184" max="184" width="5.19921875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="185" max="185" width="5.296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="186" max="186" width="4.296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="187" max="187" width="4.19921875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="188" max="188" width="4.296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="189" max="189" width="4.09765625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="190" max="190" width="4.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="191" max="191" width="5.296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="192" max="192" width="4.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="193" max="193" width="5.296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="194" max="194" width="4.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="195" max="195" width="4.296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="196" max="196" width="3.3984375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="197" max="197" width="4.59765625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="198" max="198" width="3.796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="199" max="199" width="4.09765625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="200" max="200" width="4.3984375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="201" max="201" width="2.296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="202" max="202" width="2.3984375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="203" max="203" width="2.796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="204" max="204" width="2.59765625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="205" max="205" width="3.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="206" max="207" width="3.09765625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="208" max="208" width="2.8984375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="209" max="209" width="2.69921875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="210" max="210" width="2.796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="211" max="211" width="2.8984375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="212" max="213" width="2.796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="214" max="214" width="2.69921875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="215" max="215" width="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="216" max="216" width="3.09765625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="217" max="217" width="2.796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="218" max="218" width="3.19921875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="219" max="219" width="3.09765625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="220" max="220" width="2.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="221" max="221" width="2.8984375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="222" max="222" width="2.69921875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="223" max="223" width="3.59765625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="224" max="225" width="3.19921875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="226" max="226" width="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="227" max="227" width="2.8984375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="228" max="228" width="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="229" max="229" width="3.69921875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="230" max="230" width="2.796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="231" max="231" width="3.3984375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="232" max="232" width="3.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="233" max="233" width="3.8984375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="234" max="234" width="3.09765625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="235" max="235" width="3.19921875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="236" max="236" width="3.09765625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="237" max="237" width="3.19921875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="238" max="238" width="3.09765625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="239" max="239" width="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="240" max="240" width="3.296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="241" max="241" width="2.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="242" max="243" width="3.296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="244" max="245" width="3.59765625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="246" max="247" width="2.8984375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="248" max="248" width="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="249" max="249" width="3.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="250" max="250" width="3.59765625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="30.69921875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="36.0" collapsed="true"/>
+    <col min="3" max="5" bestFit="true" customWidth="true" width="30.69921875" collapsed="true"/>
+    <col min="6" max="7" bestFit="true" customWidth="true" width="21.5" collapsed="true"/>
+    <col min="8" max="9" bestFit="true" customWidth="true" width="21.8984375" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="25.09765625" collapsed="true"/>
+    <col min="11" max="13" bestFit="true" customWidth="true" width="25.59765625" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="30.69921875" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="26.796875" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="28.796875" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="30.69921875" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="28.796875" collapsed="true"/>
+    <col min="19" max="20" bestFit="true" customWidth="true" width="30.69921875" collapsed="true"/>
+    <col min="21" max="26" bestFit="true" customWidth="true" width="28.796875" collapsed="true"/>
+    <col min="27" max="29" bestFit="true" customWidth="true" width="30.69921875" collapsed="true"/>
+    <col min="30" max="40" bestFit="true" customWidth="true" width="28.796875" collapsed="true"/>
+    <col min="41" max="41" bestFit="true" customWidth="true" width="18.8984375" collapsed="true"/>
+    <col min="42" max="43" bestFit="true" customWidth="true" width="21.796875" collapsed="true"/>
+    <col min="44" max="44" bestFit="true" customWidth="true" width="20.69921875" collapsed="true"/>
+    <col min="45" max="45" bestFit="true" customWidth="true" width="20.0" collapsed="true"/>
+    <col min="46" max="47" bestFit="true" customWidth="true" width="22.8984375" collapsed="true"/>
+    <col min="48" max="48" bestFit="true" customWidth="true" width="21.8984375" collapsed="true"/>
+    <col min="49" max="49" bestFit="true" customWidth="true" width="16.8984375" collapsed="true"/>
+    <col min="50" max="50" bestFit="true" customWidth="true" width="13.3984375" collapsed="true"/>
+    <col min="51" max="51" bestFit="true" customWidth="true" width="5.0" collapsed="true"/>
+    <col min="52" max="52" bestFit="true" customWidth="true" width="4.3984375" collapsed="true"/>
+    <col min="53" max="53" bestFit="true" customWidth="true" width="4.296875" collapsed="true"/>
+    <col min="54" max="54" bestFit="true" customWidth="true" width="4.3984375" collapsed="true"/>
+    <col min="55" max="55" bestFit="true" customWidth="true" width="4.296875" collapsed="true"/>
+    <col min="56" max="56" bestFit="true" customWidth="true" width="4.8984375" collapsed="true"/>
+    <col min="57" max="57" bestFit="true" customWidth="true" width="4.796875" collapsed="true"/>
+    <col min="58" max="58" bestFit="true" customWidth="true" width="3.796875" collapsed="true"/>
+    <col min="59" max="59" bestFit="true" customWidth="true" width="4.3984375" collapsed="true"/>
+    <col min="60" max="60" bestFit="true" customWidth="true" width="4.09765625" collapsed="true"/>
+    <col min="61" max="61" bestFit="true" customWidth="true" width="4.3984375" collapsed="true"/>
+    <col min="62" max="62" bestFit="true" customWidth="true" width="4.5" collapsed="true"/>
+    <col min="63" max="63" bestFit="true" customWidth="true" width="4.69921875" collapsed="true"/>
+    <col min="64" max="64" bestFit="true" customWidth="true" width="4.5" collapsed="true"/>
+    <col min="65" max="65" bestFit="true" customWidth="true" width="4.69921875" collapsed="true"/>
+    <col min="66" max="66" bestFit="true" customWidth="true" width="4.09765625" collapsed="true"/>
+    <col min="67" max="67" bestFit="true" customWidth="true" width="4.296875" collapsed="true"/>
+    <col min="68" max="68" bestFit="true" customWidth="true" width="4.19921875" collapsed="true"/>
+    <col min="69" max="69" bestFit="true" customWidth="true" width="4.296875" collapsed="true"/>
+    <col min="70" max="70" bestFit="true" customWidth="true" width="4.5" collapsed="true"/>
+    <col min="71" max="71" bestFit="true" customWidth="true" width="4.3984375" collapsed="true"/>
+    <col min="72" max="72" bestFit="true" customWidth="true" width="5.09765625" collapsed="true"/>
+    <col min="73" max="74" bestFit="true" customWidth="true" width="4.296875" collapsed="true"/>
+    <col min="75" max="75" bestFit="true" customWidth="true" width="4.796875" collapsed="true"/>
+    <col min="76" max="76" bestFit="true" customWidth="true" width="4.8984375" collapsed="true"/>
+    <col min="77" max="77" bestFit="true" customWidth="true" width="4.796875" collapsed="true"/>
+    <col min="78" max="78" bestFit="true" customWidth="true" width="4.8984375" collapsed="true"/>
+    <col min="79" max="80" bestFit="true" customWidth="true" width="4.796875" collapsed="true"/>
+    <col min="81" max="81" bestFit="true" customWidth="true" width="4.0" collapsed="true"/>
+    <col min="82" max="82" bestFit="true" customWidth="true" width="4.8984375" collapsed="true"/>
+    <col min="83" max="83" bestFit="true" customWidth="true" width="4.5" collapsed="true"/>
+    <col min="84" max="84" bestFit="true" customWidth="true" width="4.8984375" collapsed="true"/>
+    <col min="85" max="85" bestFit="true" customWidth="true" width="4.5" collapsed="true"/>
+    <col min="86" max="86" bestFit="true" customWidth="true" width="4.296875" collapsed="true"/>
+    <col min="87" max="87" bestFit="true" customWidth="true" width="4.09765625" collapsed="true"/>
+    <col min="88" max="88" bestFit="true" customWidth="true" width="4.3984375" collapsed="true"/>
+    <col min="89" max="91" bestFit="true" customWidth="true" width="4.796875" collapsed="true"/>
+    <col min="92" max="92" bestFit="true" customWidth="true" width="5.296875" collapsed="true"/>
+    <col min="93" max="93" bestFit="true" customWidth="true" width="4.8984375" collapsed="true"/>
+    <col min="94" max="94" bestFit="true" customWidth="true" width="5.296875" collapsed="true"/>
+    <col min="95" max="95" bestFit="true" customWidth="true" width="4.8984375" collapsed="true"/>
+    <col min="96" max="96" bestFit="true" customWidth="true" width="5.0" collapsed="true"/>
+    <col min="97" max="97" bestFit="true" customWidth="true" width="4.8984375" collapsed="true"/>
+    <col min="98" max="98" bestFit="true" customWidth="true" width="4.796875" collapsed="true"/>
+    <col min="99" max="99" bestFit="true" customWidth="true" width="5.19921875" collapsed="true"/>
+    <col min="100" max="100" bestFit="true" customWidth="true" width="4.796875" collapsed="true"/>
+    <col min="101" max="101" bestFit="true" customWidth="true" width="5.19921875" collapsed="true"/>
+    <col min="102" max="102" bestFit="true" customWidth="true" width="4.796875" collapsed="true"/>
+    <col min="103" max="103" bestFit="true" customWidth="true" width="4.8984375" collapsed="true"/>
+    <col min="104" max="104" bestFit="true" customWidth="true" width="4.296875" collapsed="true"/>
+    <col min="105" max="105" bestFit="true" customWidth="true" width="4.796875" collapsed="true"/>
+    <col min="106" max="107" bestFit="true" customWidth="true" width="4.19921875" collapsed="true"/>
+    <col min="108" max="108" bestFit="true" customWidth="true" width="4.09765625" collapsed="true"/>
+    <col min="109" max="109" bestFit="true" customWidth="true" width="4.59765625" collapsed="true"/>
+    <col min="110" max="110" bestFit="true" customWidth="true" width="4.3984375" collapsed="true"/>
+    <col min="111" max="111" bestFit="true" customWidth="true" width="4.59765625" collapsed="true"/>
+    <col min="112" max="114" bestFit="true" customWidth="true" width="4.69921875" collapsed="true"/>
+    <col min="115" max="116" bestFit="true" customWidth="true" width="4.19921875" collapsed="true"/>
+    <col min="117" max="117" bestFit="true" customWidth="true" width="4.0" collapsed="true"/>
+    <col min="118" max="119" bestFit="true" customWidth="true" width="4.19921875" collapsed="true"/>
+    <col min="120" max="121" bestFit="true" customWidth="true" width="4.5" collapsed="true"/>
+    <col min="122" max="122" bestFit="true" customWidth="true" width="4.59765625" collapsed="true"/>
+    <col min="123" max="123" bestFit="true" customWidth="true" width="4.296875" collapsed="true"/>
+    <col min="124" max="124" bestFit="true" customWidth="true" width="4.09765625" collapsed="true"/>
+    <col min="125" max="125" bestFit="true" customWidth="true" width="5.296875" collapsed="true"/>
+    <col min="126" max="126" bestFit="true" customWidth="true" width="4.3984375" collapsed="true"/>
+    <col min="127" max="127" bestFit="true" customWidth="true" width="5.296875" collapsed="true"/>
+    <col min="128" max="128" bestFit="true" customWidth="true" width="4.8984375" collapsed="true"/>
+    <col min="129" max="129" bestFit="true" customWidth="true" width="4.59765625" collapsed="true"/>
+    <col min="130" max="130" bestFit="true" customWidth="true" width="4.5" collapsed="true"/>
+    <col min="131" max="131" bestFit="true" customWidth="true" width="4.796875" collapsed="true"/>
+    <col min="132" max="133" bestFit="true" customWidth="true" width="4.5" collapsed="true"/>
+    <col min="134" max="134" bestFit="true" customWidth="true" width="4.3984375" collapsed="true"/>
+    <col min="135" max="135" bestFit="true" customWidth="true" width="4.59765625" collapsed="true"/>
+    <col min="136" max="136" bestFit="true" customWidth="true" width="4.3984375" collapsed="true"/>
+    <col min="137" max="137" bestFit="true" customWidth="true" width="4.59765625" collapsed="true"/>
+    <col min="138" max="138" bestFit="true" customWidth="true" width="4.796875" collapsed="true"/>
+    <col min="139" max="141" bestFit="true" customWidth="true" width="4.8984375" collapsed="true"/>
+    <col min="142" max="142" bestFit="true" customWidth="true" width="4.59765625" collapsed="true"/>
+    <col min="143" max="143" bestFit="true" customWidth="true" width="4.19921875" collapsed="true"/>
+    <col min="144" max="144" bestFit="true" customWidth="true" width="4.59765625" collapsed="true"/>
+    <col min="145" max="145" bestFit="true" customWidth="true" width="4.3984375" collapsed="true"/>
+    <col min="146" max="146" bestFit="true" customWidth="true" width="5.0" collapsed="true"/>
+    <col min="147" max="147" bestFit="true" customWidth="true" width="4.3984375" collapsed="true"/>
+    <col min="148" max="148" bestFit="true" customWidth="true" width="5.0" collapsed="true"/>
+    <col min="149" max="149" bestFit="true" customWidth="true" width="4.3984375" collapsed="true"/>
+    <col min="150" max="150" bestFit="true" customWidth="true" width="4.796875" collapsed="true"/>
+    <col min="151" max="151" bestFit="true" customWidth="true" width="4.296875" collapsed="true"/>
+    <col min="152" max="152" bestFit="true" customWidth="true" width="4.796875" collapsed="true"/>
+    <col min="153" max="153" bestFit="true" customWidth="true" width="4.296875" collapsed="true"/>
+    <col min="154" max="154" bestFit="true" customWidth="true" width="4.796875" collapsed="true"/>
+    <col min="155" max="156" bestFit="true" customWidth="true" width="4.296875" collapsed="true"/>
+    <col min="157" max="157" bestFit="true" customWidth="true" width="4.3984375" collapsed="true"/>
+    <col min="158" max="158" bestFit="true" customWidth="true" width="4.09765625" collapsed="true"/>
+    <col min="159" max="159" bestFit="true" customWidth="true" width="3.796875" collapsed="true"/>
+    <col min="160" max="160" bestFit="true" customWidth="true" width="4.19921875" collapsed="true"/>
+    <col min="161" max="161" bestFit="true" customWidth="true" width="4.8984375" collapsed="true"/>
+    <col min="162" max="162" bestFit="true" customWidth="true" width="3.796875" collapsed="true"/>
+    <col min="163" max="163" bestFit="true" customWidth="true" width="4.8984375" collapsed="true"/>
+    <col min="164" max="165" bestFit="true" customWidth="true" width="5.0" collapsed="true"/>
+    <col min="166" max="166" bestFit="true" customWidth="true" width="5.3984375" collapsed="true"/>
+    <col min="167" max="167" bestFit="true" customWidth="true" width="5.0" collapsed="true"/>
+    <col min="168" max="168" bestFit="true" customWidth="true" width="5.3984375" collapsed="true"/>
+    <col min="169" max="169" bestFit="true" customWidth="true" width="4.69921875" collapsed="true"/>
+    <col min="170" max="170" bestFit="true" customWidth="true" width="4.59765625" collapsed="true"/>
+    <col min="171" max="171" bestFit="true" customWidth="true" width="4.296875" collapsed="true"/>
+    <col min="172" max="172" bestFit="true" customWidth="true" width="5.0" collapsed="true"/>
+    <col min="173" max="173" bestFit="true" customWidth="true" width="4.5" collapsed="true"/>
+    <col min="174" max="174" bestFit="true" customWidth="true" width="5.19921875" collapsed="true"/>
+    <col min="175" max="175" bestFit="true" customWidth="true" width="4.5" collapsed="true"/>
+    <col min="176" max="176" bestFit="true" customWidth="true" width="4.8984375" collapsed="true"/>
+    <col min="177" max="177" bestFit="true" customWidth="true" width="5.0" collapsed="true"/>
+    <col min="178" max="178" bestFit="true" customWidth="true" width="4.69921875" collapsed="true"/>
+    <col min="179" max="179" bestFit="true" customWidth="true" width="4.19921875" collapsed="true"/>
+    <col min="180" max="180" bestFit="true" customWidth="true" width="4.3984375" collapsed="true"/>
+    <col min="181" max="181" bestFit="true" customWidth="true" width="4.19921875" collapsed="true"/>
+    <col min="182" max="182" bestFit="true" customWidth="true" width="4.3984375" collapsed="true"/>
+    <col min="183" max="183" bestFit="true" customWidth="true" width="4.296875" collapsed="true"/>
+    <col min="184" max="184" bestFit="true" customWidth="true" width="5.19921875" collapsed="true"/>
+    <col min="185" max="185" bestFit="true" customWidth="true" width="5.296875" collapsed="true"/>
+    <col min="186" max="186" bestFit="true" customWidth="true" width="4.296875" collapsed="true"/>
+    <col min="187" max="187" bestFit="true" customWidth="true" width="4.19921875" collapsed="true"/>
+    <col min="188" max="188" bestFit="true" customWidth="true" width="4.296875" collapsed="true"/>
+    <col min="189" max="189" bestFit="true" customWidth="true" width="4.09765625" collapsed="true"/>
+    <col min="190" max="190" bestFit="true" customWidth="true" width="4.5" collapsed="true"/>
+    <col min="191" max="191" bestFit="true" customWidth="true" width="5.296875" collapsed="true"/>
+    <col min="192" max="192" bestFit="true" customWidth="true" width="4.5" collapsed="true"/>
+    <col min="193" max="193" bestFit="true" customWidth="true" width="5.296875" collapsed="true"/>
+    <col min="194" max="194" bestFit="true" customWidth="true" width="4.5" collapsed="true"/>
+    <col min="195" max="195" bestFit="true" customWidth="true" width="4.296875" collapsed="true"/>
+    <col min="196" max="196" bestFit="true" customWidth="true" width="3.3984375" collapsed="true"/>
+    <col min="197" max="197" bestFit="true" customWidth="true" width="4.59765625" collapsed="true"/>
+    <col min="198" max="198" bestFit="true" customWidth="true" width="3.796875" collapsed="true"/>
+    <col min="199" max="199" bestFit="true" customWidth="true" width="4.09765625" collapsed="true"/>
+    <col min="200" max="200" bestFit="true" customWidth="true" width="4.3984375" collapsed="true"/>
+    <col min="201" max="201" bestFit="true" customWidth="true" width="2.296875" collapsed="true"/>
+    <col min="202" max="202" bestFit="true" customWidth="true" width="2.3984375" collapsed="true"/>
+    <col min="203" max="203" bestFit="true" customWidth="true" width="2.796875" collapsed="true"/>
+    <col min="204" max="204" bestFit="true" customWidth="true" width="2.59765625" collapsed="true"/>
+    <col min="205" max="205" bestFit="true" customWidth="true" width="3.5" collapsed="true"/>
+    <col min="206" max="207" bestFit="true" customWidth="true" width="3.09765625" collapsed="true"/>
+    <col min="208" max="208" bestFit="true" customWidth="true" width="2.8984375" collapsed="true"/>
+    <col min="209" max="209" bestFit="true" customWidth="true" width="2.69921875" collapsed="true"/>
+    <col min="210" max="210" bestFit="true" customWidth="true" width="2.796875" collapsed="true"/>
+    <col min="211" max="211" bestFit="true" customWidth="true" width="2.8984375" collapsed="true"/>
+    <col min="212" max="213" bestFit="true" customWidth="true" width="2.796875" collapsed="true"/>
+    <col min="214" max="214" bestFit="true" customWidth="true" width="2.69921875" collapsed="true"/>
+    <col min="215" max="215" bestFit="true" customWidth="true" width="3.0" collapsed="true"/>
+    <col min="216" max="216" bestFit="true" customWidth="true" width="3.09765625" collapsed="true"/>
+    <col min="217" max="217" bestFit="true" customWidth="true" width="2.796875" collapsed="true"/>
+    <col min="218" max="218" bestFit="true" customWidth="true" width="3.19921875" collapsed="true"/>
+    <col min="219" max="219" bestFit="true" customWidth="true" width="3.09765625" collapsed="true"/>
+    <col min="220" max="220" bestFit="true" customWidth="true" width="2.5" collapsed="true"/>
+    <col min="221" max="221" bestFit="true" customWidth="true" width="2.8984375" collapsed="true"/>
+    <col min="222" max="222" bestFit="true" customWidth="true" width="2.69921875" collapsed="true"/>
+    <col min="223" max="223" bestFit="true" customWidth="true" width="3.59765625" collapsed="true"/>
+    <col min="224" max="225" bestFit="true" customWidth="true" width="3.19921875" collapsed="true"/>
+    <col min="226" max="226" bestFit="true" customWidth="true" width="3.0" collapsed="true"/>
+    <col min="227" max="227" bestFit="true" customWidth="true" width="2.8984375" collapsed="true"/>
+    <col min="228" max="228" bestFit="true" customWidth="true" width="3.0" collapsed="true"/>
+    <col min="229" max="229" bestFit="true" customWidth="true" width="3.69921875" collapsed="true"/>
+    <col min="230" max="230" bestFit="true" customWidth="true" width="2.796875" collapsed="true"/>
+    <col min="231" max="231" bestFit="true" customWidth="true" width="3.3984375" collapsed="true"/>
+    <col min="232" max="232" bestFit="true" customWidth="true" width="3.5" collapsed="true"/>
+    <col min="233" max="233" bestFit="true" customWidth="true" width="3.8984375" collapsed="true"/>
+    <col min="234" max="234" bestFit="true" customWidth="true" width="3.09765625" collapsed="true"/>
+    <col min="235" max="235" bestFit="true" customWidth="true" width="3.19921875" collapsed="true"/>
+    <col min="236" max="236" bestFit="true" customWidth="true" width="3.09765625" collapsed="true"/>
+    <col min="237" max="237" bestFit="true" customWidth="true" width="3.19921875" collapsed="true"/>
+    <col min="238" max="238" bestFit="true" customWidth="true" width="3.09765625" collapsed="true"/>
+    <col min="239" max="239" bestFit="true" customWidth="true" width="3.0" collapsed="true"/>
+    <col min="240" max="240" bestFit="true" customWidth="true" width="3.296875" collapsed="true"/>
+    <col min="241" max="241" bestFit="true" customWidth="true" width="2.5" collapsed="true"/>
+    <col min="242" max="243" bestFit="true" customWidth="true" width="3.296875" collapsed="true"/>
+    <col min="244" max="245" bestFit="true" customWidth="true" width="3.59765625" collapsed="true"/>
+    <col min="246" max="247" bestFit="true" customWidth="true" width="2.8984375" collapsed="true"/>
+    <col min="248" max="248" bestFit="true" customWidth="true" width="3.0" collapsed="true"/>
+    <col min="249" max="249" bestFit="true" customWidth="true" width="3.5" collapsed="true"/>
+    <col min="250" max="250" bestFit="true" customWidth="true" width="3.59765625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:50" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Updated Failed TC and completed TS83
</commit_message>
<xml_diff>
--- a/src/main/resources/Bulk_ConventionalTransactions_File.xlsx
+++ b/src/main/resources/Bulk_ConventionalTransactions_File.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24405" uniqueCount="665">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24411" uniqueCount="670">
   <si>
     <t>transactionName</t>
   </si>
@@ -2016,6 +2016,21 @@
   <si>
     <t>01.46 PM</t>
   </si>
+  <si>
+    <t>tran7863676605</t>
+  </si>
+  <si>
+    <t>transaction17863676605</t>
+  </si>
+  <si>
+    <t>4852527582</t>
+  </si>
+  <si>
+    <t>2243684335</t>
+  </si>
+  <si>
+    <t>11.37 AM</t>
+  </si>
 </sst>
 </file>
 
@@ -2800,10 +2815,10 @@
     </row>
     <row r="2" spans="1:97" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>660</v>
+        <v>665</v>
       </c>
       <c r="B2" t="s">
-        <v>662</v>
+        <v>667</v>
       </c>
       <c r="C2" t="s">
         <v>488</v>
@@ -2863,7 +2878,7 @@
         <v>109</v>
       </c>
       <c r="V2" t="s">
-        <v>664</v>
+        <v>669</v>
       </c>
       <c r="W2" s="1" t="s">
         <v>103</v>
@@ -3061,10 +3076,10 @@
     </row>
     <row r="3" spans="1:97" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>661</v>
+        <v>666</v>
       </c>
       <c r="B3" t="s">
-        <v>663</v>
+        <v>668</v>
       </c>
       <c r="C3" t="s">
         <v>488</v>
@@ -3085,7 +3100,7 @@
         <v>109</v>
       </c>
       <c r="V3" t="s">
-        <v>664</v>
+        <v>669</v>
       </c>
       <c r="W3" s="1" t="s">
         <v>103</v>

</xml_diff>

<commit_message>
Updated TS13 and TS27
</commit_message>
<xml_diff>
--- a/src/main/resources/Bulk_ConventionalTransactions_File.xlsx
+++ b/src/main/resources/Bulk_ConventionalTransactions_File.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24447" uniqueCount="700">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24477" uniqueCount="725">
   <si>
     <t>transactionName</t>
   </si>
@@ -2121,6 +2121,81 @@
   <si>
     <t>12.52 PM</t>
   </si>
+  <si>
+    <t>tran5105728228</t>
+  </si>
+  <si>
+    <t>transaction15105728228</t>
+  </si>
+  <si>
+    <t>6451599200</t>
+  </si>
+  <si>
+    <t>3153428824</t>
+  </si>
+  <si>
+    <t>11.12 AM</t>
+  </si>
+  <si>
+    <t>tran3814018247</t>
+  </si>
+  <si>
+    <t>transaction13814018247</t>
+  </si>
+  <si>
+    <t>6510260101</t>
+  </si>
+  <si>
+    <t>8160920283</t>
+  </si>
+  <si>
+    <t>05.57 PM</t>
+  </si>
+  <si>
+    <t>tran4791195695</t>
+  </si>
+  <si>
+    <t>transaction14791195695</t>
+  </si>
+  <si>
+    <t>6664213389</t>
+  </si>
+  <si>
+    <t>4877916348</t>
+  </si>
+  <si>
+    <t>09.45 AM</t>
+  </si>
+  <si>
+    <t>tran6013879990</t>
+  </si>
+  <si>
+    <t>transaction16013879990</t>
+  </si>
+  <si>
+    <t>4869506858</t>
+  </si>
+  <si>
+    <t>5844718010</t>
+  </si>
+  <si>
+    <t>10.24 AM</t>
+  </si>
+  <si>
+    <t>tran6275054905</t>
+  </si>
+  <si>
+    <t>transaction16275054905</t>
+  </si>
+  <si>
+    <t>7158038961</t>
+  </si>
+  <si>
+    <t>8803321960</t>
+  </si>
+  <si>
+    <t>11.20 AM</t>
+  </si>
 </sst>
 </file>
 
@@ -2905,10 +2980,10 @@
     </row>
     <row r="2" spans="1:97" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>695</v>
+        <v>720</v>
       </c>
       <c r="B2" t="s">
-        <v>697</v>
+        <v>722</v>
       </c>
       <c r="C2" t="s">
         <v>488</v>
@@ -2968,7 +3043,7 @@
         <v>109</v>
       </c>
       <c r="V2" t="s">
-        <v>699</v>
+        <v>724</v>
       </c>
       <c r="W2" s="1" t="s">
         <v>103</v>
@@ -3166,10 +3241,10 @@
     </row>
     <row r="3" spans="1:97" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>696</v>
+        <v>721</v>
       </c>
       <c r="B3" t="s">
-        <v>698</v>
+        <v>723</v>
       </c>
       <c r="C3" t="s">
         <v>488</v>
@@ -3190,7 +3265,7 @@
         <v>109</v>
       </c>
       <c r="V3" t="s">
-        <v>699</v>
+        <v>724</v>
       </c>
       <c r="W3" s="1" t="s">
         <v>103</v>

</xml_diff>

<commit_message>
Completed Test case 106
</commit_message>
<xml_diff>
--- a/src/main/resources/Bulk_ConventionalTransactions_File.xlsx
+++ b/src/main/resources/Bulk_ConventionalTransactions_File.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24483" uniqueCount="730">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24489" uniqueCount="735">
   <si>
     <t>transactionName</t>
   </si>
@@ -2211,6 +2211,21 @@
   <si>
     <t>12.37 PM</t>
   </si>
+  <si>
+    <t>tran8372133763</t>
+  </si>
+  <si>
+    <t>transaction18372133763</t>
+  </si>
+  <si>
+    <t>5109905583</t>
+  </si>
+  <si>
+    <t>6242482662</t>
+  </si>
+  <si>
+    <t>01.21 PM</t>
+  </si>
 </sst>
 </file>
 
@@ -2995,10 +3010,10 @@
     </row>
     <row r="2" spans="1:97" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>725</v>
+        <v>730</v>
       </c>
       <c r="B2" t="s">
-        <v>727</v>
+        <v>732</v>
       </c>
       <c r="C2" t="s">
         <v>488</v>
@@ -3058,7 +3073,7 @@
         <v>109</v>
       </c>
       <c r="V2" t="s">
-        <v>729</v>
+        <v>734</v>
       </c>
       <c r="W2" s="1" t="s">
         <v>103</v>
@@ -3256,10 +3271,10 @@
     </row>
     <row r="3" spans="1:97" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>726</v>
+        <v>731</v>
       </c>
       <c r="B3" t="s">
-        <v>728</v>
+        <v>733</v>
       </c>
       <c r="C3" t="s">
         <v>488</v>
@@ -3280,7 +3295,7 @@
         <v>109</v>
       </c>
       <c r="V3" t="s">
-        <v>729</v>
+        <v>734</v>
       </c>
       <c r="W3" s="1" t="s">
         <v>103</v>

</xml_diff>

<commit_message>
edited failed test cases
</commit_message>
<xml_diff>
--- a/src/main/resources/Bulk_ConventionalTransactions_File.xlsx
+++ b/src/main/resources/Bulk_ConventionalTransactions_File.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24489" uniqueCount="735">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24507" uniqueCount="750">
   <si>
     <t>transactionName</t>
   </si>
@@ -2226,6 +2226,51 @@
   <si>
     <t>01.21 PM</t>
   </si>
+  <si>
+    <t>tran9917053310</t>
+  </si>
+  <si>
+    <t>transaction19917053310</t>
+  </si>
+  <si>
+    <t>4578894423</t>
+  </si>
+  <si>
+    <t>5083501852</t>
+  </si>
+  <si>
+    <t>04.00 PM</t>
+  </si>
+  <si>
+    <t>tran6526992040</t>
+  </si>
+  <si>
+    <t>transaction16526992040</t>
+  </si>
+  <si>
+    <t>6792387700</t>
+  </si>
+  <si>
+    <t>6246209668</t>
+  </si>
+  <si>
+    <t>04.08 PM</t>
+  </si>
+  <si>
+    <t>tran6099935064</t>
+  </si>
+  <si>
+    <t>transaction16099935064</t>
+  </si>
+  <si>
+    <t>1359472530</t>
+  </si>
+  <si>
+    <t>4842217831</t>
+  </si>
+  <si>
+    <t>04.16 PM</t>
+  </si>
 </sst>
 </file>
 
@@ -3010,10 +3055,10 @@
     </row>
     <row r="2" spans="1:97" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>730</v>
+        <v>745</v>
       </c>
       <c r="B2" t="s">
-        <v>732</v>
+        <v>747</v>
       </c>
       <c r="C2" t="s">
         <v>488</v>
@@ -3073,7 +3118,7 @@
         <v>109</v>
       </c>
       <c r="V2" t="s">
-        <v>734</v>
+        <v>749</v>
       </c>
       <c r="W2" s="1" t="s">
         <v>103</v>
@@ -3271,10 +3316,10 @@
     </row>
     <row r="3" spans="1:97" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>731</v>
+        <v>746</v>
       </c>
       <c r="B3" t="s">
-        <v>733</v>
+        <v>748</v>
       </c>
       <c r="C3" t="s">
         <v>488</v>
@@ -3295,7 +3340,7 @@
         <v>109</v>
       </c>
       <c r="V3" t="s">
-        <v>734</v>
+        <v>749</v>
       </c>
       <c r="W3" s="1" t="s">
         <v>103</v>

</xml_diff>

<commit_message>
Updated Failed 37 and 27 test cases
</commit_message>
<xml_diff>
--- a/src/main/resources/Bulk_ConventionalTransactions_File.xlsx
+++ b/src/main/resources/Bulk_ConventionalTransactions_File.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\BDD_Framework\30 March\10MayNew\29May-Main\9Oct\upp-test-automation\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24399" uniqueCount="660">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24429" uniqueCount="684">
   <si>
     <t>transactionName</t>
   </si>
@@ -1960,46 +1960,118 @@
     <t>SCBLINBB</t>
   </si>
   <si>
-    <t>ADD1</t>
-  </si>
-  <si>
     <t>ADD2</t>
   </si>
   <si>
-    <t>ACCRAK132</t>
+    <t>tran3908076670</t>
   </si>
   <si>
-    <t>ACCRAK1867</t>
+    <t>transaction13908076670</t>
   </si>
   <si>
-    <t>tran8653227731</t>
+    <t>3722303930</t>
   </si>
   <si>
-    <t>transaction18653227731</t>
+    <t>6993615013</t>
   </si>
   <si>
-    <t>2369729480</t>
+    <t>11.20 AM</t>
   </si>
   <si>
-    <t>8867573668</t>
+    <t>ACCRAK1868</t>
   </si>
   <si>
-    <t>03.39 PM</t>
+    <t>ACCRAK1327</t>
   </si>
   <si>
-    <t>tran7775271136</t>
+    <t>ADD3</t>
   </si>
   <si>
-    <t>transaction17775271136</t>
+    <t>tran8240935293</t>
   </si>
   <si>
-    <t>9014569087</t>
+    <t>transaction18240935293</t>
   </si>
   <si>
-    <t>4975330404</t>
+    <t>5642006359</t>
   </si>
   <si>
-    <t>06.09 PM</t>
+    <t>8631169213</t>
+  </si>
+  <si>
+    <t>11.45 AM</t>
+  </si>
+  <si>
+    <t>tran8379587651</t>
+  </si>
+  <si>
+    <t>transaction18379587651</t>
+  </si>
+  <si>
+    <t>5034255779</t>
+  </si>
+  <si>
+    <t>1668976285</t>
+  </si>
+  <si>
+    <t>12.25 PM</t>
+  </si>
+  <si>
+    <t>tran9404191945</t>
+  </si>
+  <si>
+    <t>transaction19404191945</t>
+  </si>
+  <si>
+    <t>8826774734</t>
+  </si>
+  <si>
+    <t>1869296936</t>
+  </si>
+  <si>
+    <t>06.05 PM</t>
+  </si>
+  <si>
+    <t>tran9516711915</t>
+  </si>
+  <si>
+    <t>transaction19516711915</t>
+  </si>
+  <si>
+    <t>9391224785</t>
+  </si>
+  <si>
+    <t>1555366948</t>
+  </si>
+  <si>
+    <t>tran2250786786</t>
+  </si>
+  <si>
+    <t>transaction12250786786</t>
+  </si>
+  <si>
+    <t>9544172509</t>
+  </si>
+  <si>
+    <t>9024598474</t>
+  </si>
+  <si>
+    <t>06.27 PM</t>
+  </si>
+  <si>
+    <t>tran2427763304</t>
+  </si>
+  <si>
+    <t>transaction12427763304</t>
+  </si>
+  <si>
+    <t>1092486528</t>
+  </si>
+  <si>
+    <t>3507109927</t>
+  </si>
+  <si>
+    <t>06.41 PM</t>
   </si>
 </sst>
 </file>
@@ -2393,8 +2465,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CS3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="Y3" sqref="Y3"/>
+    <sheetView tabSelected="1" topLeftCell="BF1" workbookViewId="0">
+      <selection activeCell="BL3" sqref="BL3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -2785,10 +2857,10 @@
     </row>
     <row r="2" spans="1:97" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>655</v>
+        <v>679</v>
       </c>
       <c r="B2" t="s">
-        <v>657</v>
+        <v>681</v>
       </c>
       <c r="C2" t="s">
         <v>488</v>
@@ -2848,7 +2920,7 @@
         <v>109</v>
       </c>
       <c r="V2" t="s">
-        <v>659</v>
+        <v>683</v>
       </c>
       <c r="W2" s="1" t="s">
         <v>103</v>
@@ -2857,7 +2929,7 @@
         <v>97</v>
       </c>
       <c r="Y2" s="1">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="Z2" s="1" t="s">
         <v>645</v>
@@ -2873,7 +2945,7 @@
       </c>
       <c r="AD2" s="2"/>
       <c r="AE2" s="1" t="s">
-        <v>649</v>
+        <v>652</v>
       </c>
       <c r="AF2" t="s">
         <v>97</v>
@@ -2897,7 +2969,7 @@
         <v>646</v>
       </c>
       <c r="AM2" s="1" t="s">
-        <v>647</v>
+        <v>654</v>
       </c>
       <c r="AN2" s="3" t="s">
         <v>488</v>
@@ -3046,10 +3118,10 @@
     </row>
     <row r="3" spans="1:97" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>656</v>
+        <v>680</v>
       </c>
       <c r="B3" t="s">
-        <v>658</v>
+        <v>682</v>
       </c>
       <c r="C3" t="s">
         <v>488</v>
@@ -3070,13 +3142,13 @@
         <v>109</v>
       </c>
       <c r="V3" t="s">
-        <v>659</v>
+        <v>683</v>
       </c>
       <c r="W3" s="1" t="s">
         <v>103</v>
       </c>
       <c r="Y3" s="1">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="Z3" s="1" t="s">
         <v>645</v>
@@ -3089,13 +3161,13 @@
       </c>
       <c r="AD3" s="2"/>
       <c r="AE3" s="1" t="s">
-        <v>648</v>
+        <v>653</v>
       </c>
       <c r="AL3" s="1" t="s">
         <v>646</v>
       </c>
       <c r="AM3" s="1" t="s">
-        <v>647</v>
+        <v>654</v>
       </c>
       <c r="AN3" s="3" t="s">
         <v>488</v>
@@ -3132,7 +3204,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:J1 F2:J2 L1:U1 L2:R2 T2 X2 AA2 AF2:AK2 BE2:BR2 BT2 BV2:CO2 CQ2:CS2 V2 W1:CS1" numberStoredAsText="1"/>
+    <ignoredError sqref="A1:J1 F2:J2 L1:U1 L2:R2 T2 X2 AA2 AF2:AK2 BE2:BR2 BT2 BV2:CO2 CQ2:CS2 W1:CS1" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Updated 27 test case
</commit_message>
<xml_diff>
--- a/src/main/resources/Bulk_ConventionalTransactions_File.xlsx
+++ b/src/main/resources/Bulk_ConventionalTransactions_File.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24488" uniqueCount="734">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24530" uniqueCount="769">
   <si>
     <t>transactionName</t>
   </si>
@@ -2223,6 +2223,111 @@
   <si>
     <t>11.47 AM</t>
   </si>
+  <si>
+    <t>tran7489932695</t>
+  </si>
+  <si>
+    <t>transaction17489932695</t>
+  </si>
+  <si>
+    <t>7496801538</t>
+  </si>
+  <si>
+    <t>6668110401</t>
+  </si>
+  <si>
+    <t>10.22 AM</t>
+  </si>
+  <si>
+    <t>tran8091203017</t>
+  </si>
+  <si>
+    <t>transaction18091203017</t>
+  </si>
+  <si>
+    <t>4699107569</t>
+  </si>
+  <si>
+    <t>4407876632</t>
+  </si>
+  <si>
+    <t>10.44 AM</t>
+  </si>
+  <si>
+    <t>tran6648717508</t>
+  </si>
+  <si>
+    <t>transaction16648717508</t>
+  </si>
+  <si>
+    <t>2218190426</t>
+  </si>
+  <si>
+    <t>3947572804</t>
+  </si>
+  <si>
+    <t>10.57 AM</t>
+  </si>
+  <si>
+    <t>tran3960952692</t>
+  </si>
+  <si>
+    <t>transaction13960952692</t>
+  </si>
+  <si>
+    <t>2888213631</t>
+  </si>
+  <si>
+    <t>3046133329</t>
+  </si>
+  <si>
+    <t>11.03 AM</t>
+  </si>
+  <si>
+    <t>tran7948168480</t>
+  </si>
+  <si>
+    <t>transaction17948168480</t>
+  </si>
+  <si>
+    <t>3520619702</t>
+  </si>
+  <si>
+    <t>7073974788</t>
+  </si>
+  <si>
+    <t>11.09 AM</t>
+  </si>
+  <si>
+    <t>tran6490486962</t>
+  </si>
+  <si>
+    <t>transaction16490486962</t>
+  </si>
+  <si>
+    <t>5399550501</t>
+  </si>
+  <si>
+    <t>1781489870</t>
+  </si>
+  <si>
+    <t>11.30 AM</t>
+  </si>
+  <si>
+    <t>tran9650383448</t>
+  </si>
+  <si>
+    <t>transaction19650383448</t>
+  </si>
+  <si>
+    <t>3780550546</t>
+  </si>
+  <si>
+    <t>6451863160</t>
+  </si>
+  <si>
+    <t>12.05 PM</t>
+  </si>
 </sst>
 </file>
 
@@ -3007,10 +3112,10 @@
     </row>
     <row r="2" spans="1:97" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>729</v>
+        <v>764</v>
       </c>
       <c r="B2" t="s">
-        <v>731</v>
+        <v>766</v>
       </c>
       <c r="C2" t="s">
         <v>488</v>
@@ -3070,7 +3175,7 @@
         <v>109</v>
       </c>
       <c r="V2" t="s">
-        <v>733</v>
+        <v>768</v>
       </c>
       <c r="W2" s="1" t="s">
         <v>103</v>
@@ -3268,10 +3373,10 @@
     </row>
     <row r="3" spans="1:97" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>730</v>
+        <v>765</v>
       </c>
       <c r="B3" t="s">
-        <v>732</v>
+        <v>767</v>
       </c>
       <c r="C3" t="s">
         <v>488</v>
@@ -3292,7 +3397,7 @@
         <v>109</v>
       </c>
       <c r="V3" t="s">
-        <v>733</v>
+        <v>768</v>
       </c>
       <c r="W3" s="1" t="s">
         <v>103</v>

</xml_diff>

<commit_message>
Updated 118 and created TS121,125
</commit_message>
<xml_diff>
--- a/src/main/resources/Bulk_ConventionalTransactions_File.xlsx
+++ b/src/main/resources/Bulk_ConventionalTransactions_File.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\BDD_Framework\30 March\10MayNew\upp-test-automation\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\BDD_Framework\30 March\10MayNew\29May-Main\9Oct\upp-test-automation\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24530" uniqueCount="769">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24400" uniqueCount="662">
   <si>
     <t>transactionName</t>
   </si>
@@ -1972,361 +1972,40 @@
     <t>ACCRAK1867</t>
   </si>
   <si>
-    <t>tran2824492469</t>
+    <t>tran8456928681</t>
   </si>
   <si>
-    <t>transaction12824492469</t>
+    <t>transaction18456928681</t>
   </si>
   <si>
-    <t>8188244029</t>
+    <t>1257282089</t>
   </si>
   <si>
-    <t>1987511998</t>
+    <t>6972999134</t>
   </si>
   <si>
-    <t>tran4900991552</t>
+    <t>12.54 PM</t>
   </si>
   <si>
-    <t>transaction14900991552</t>
+    <t>SBI463</t>
   </si>
   <si>
-    <t>9053892786</t>
+    <t>SBI4634324</t>
   </si>
   <si>
-    <t>1872364902</t>
+    <t>tran1810945966</t>
   </si>
   <si>
-    <t>11.37 AM</t>
+    <t>transaction11810945966</t>
   </si>
   <si>
-    <t>tran5751985401</t>
+    <t>2568211673</t>
   </si>
   <si>
-    <t>transaction15751985401</t>
+    <t>8705192721</t>
   </si>
   <si>
-    <t>2553774071</t>
-  </si>
-  <si>
-    <t>4814091974</t>
-  </si>
-  <si>
-    <t>12.18 PM</t>
-  </si>
-  <si>
-    <t>tran6515111970</t>
-  </si>
-  <si>
-    <t>transaction16515111970</t>
-  </si>
-  <si>
-    <t>7846345842</t>
-  </si>
-  <si>
-    <t>5212267249</t>
-  </si>
-  <si>
-    <t>12.57 PM</t>
-  </si>
-  <si>
-    <t>tran4260025472</t>
-  </si>
-  <si>
-    <t>transaction14260025472</t>
-  </si>
-  <si>
-    <t>2222959970</t>
-  </si>
-  <si>
-    <t>4169697419</t>
-  </si>
-  <si>
-    <t>01.05 PM</t>
-  </si>
-  <si>
-    <t>tran2961849940</t>
-  </si>
-  <si>
-    <t>transaction12961849940</t>
-  </si>
-  <si>
-    <t>5968735885</t>
-  </si>
-  <si>
-    <t>2709705659</t>
-  </si>
-  <si>
-    <t>01.16 PM</t>
-  </si>
-  <si>
-    <t>tran4965433832</t>
-  </si>
-  <si>
-    <t>transaction14965433832</t>
-  </si>
-  <si>
-    <t>8037772175</t>
-  </si>
-  <si>
-    <t>8046481903</t>
-  </si>
-  <si>
-    <t>02.35 PM</t>
-  </si>
-  <si>
-    <t>tran7083747862</t>
-  </si>
-  <si>
-    <t>transaction17083747862</t>
-  </si>
-  <si>
-    <t>8382692307</t>
-  </si>
-  <si>
-    <t>3679862499</t>
-  </si>
-  <si>
-    <t>03.51 PM</t>
-  </si>
-  <si>
-    <t>tran3800447970</t>
-  </si>
-  <si>
-    <t>transaction13800447970</t>
-  </si>
-  <si>
-    <t>1927934092</t>
-  </si>
-  <si>
-    <t>3163916840</t>
-  </si>
-  <si>
-    <t>04.05 PM</t>
-  </si>
-  <si>
-    <t>tran9609146007</t>
-  </si>
-  <si>
-    <t>transaction19609146007</t>
-  </si>
-  <si>
-    <t>1444715759</t>
-  </si>
-  <si>
-    <t>3099884742</t>
-  </si>
-  <si>
-    <t>04.08 PM</t>
-  </si>
-  <si>
-    <t>tran4598281393</t>
-  </si>
-  <si>
-    <t>transaction14598281393</t>
-  </si>
-  <si>
-    <t>3865389061</t>
-  </si>
-  <si>
-    <t>9591483918</t>
-  </si>
-  <si>
-    <t>05.46 PM</t>
-  </si>
-  <si>
-    <t>tran2067055416</t>
-  </si>
-  <si>
-    <t>transaction12067055416</t>
-  </si>
-  <si>
-    <t>2310048982</t>
-  </si>
-  <si>
-    <t>7211318695</t>
-  </si>
-  <si>
-    <t>05.58 PM</t>
-  </si>
-  <si>
-    <t>tran1580889644</t>
-  </si>
-  <si>
-    <t>transaction11580889644</t>
-  </si>
-  <si>
-    <t>1536157811</t>
-  </si>
-  <si>
-    <t>9979000024</t>
-  </si>
-  <si>
-    <t>10.16 AM</t>
-  </si>
-  <si>
-    <t>tran8231494953</t>
-  </si>
-  <si>
-    <t>transaction18231494953</t>
-  </si>
-  <si>
-    <t>2977110997</t>
-  </si>
-  <si>
-    <t>1574214716</t>
-  </si>
-  <si>
-    <t>05.00 PM</t>
-  </si>
-  <si>
-    <t>tran2035892075</t>
-  </si>
-  <si>
-    <t>transaction12035892075</t>
-  </si>
-  <si>
-    <t>3796723388</t>
-  </si>
-  <si>
-    <t>9236412898</t>
-  </si>
-  <si>
-    <t>05.29 PM</t>
-  </si>
-  <si>
-    <t>tran5002980012</t>
-  </si>
-  <si>
-    <t>transaction15002980012</t>
-  </si>
-  <si>
-    <t>8099308384</t>
-  </si>
-  <si>
-    <t>8142655474</t>
-  </si>
-  <si>
-    <t>05.54 PM</t>
-  </si>
-  <si>
-    <t>tran4084658186</t>
-  </si>
-  <si>
-    <t>transaction14084658186</t>
-  </si>
-  <si>
-    <t>1787168962</t>
-  </si>
-  <si>
-    <t>3048550635</t>
-  </si>
-  <si>
-    <t>11.47 AM</t>
-  </si>
-  <si>
-    <t>tran7489932695</t>
-  </si>
-  <si>
-    <t>transaction17489932695</t>
-  </si>
-  <si>
-    <t>7496801538</t>
-  </si>
-  <si>
-    <t>6668110401</t>
-  </si>
-  <si>
-    <t>10.22 AM</t>
-  </si>
-  <si>
-    <t>tran8091203017</t>
-  </si>
-  <si>
-    <t>transaction18091203017</t>
-  </si>
-  <si>
-    <t>4699107569</t>
-  </si>
-  <si>
-    <t>4407876632</t>
-  </si>
-  <si>
-    <t>10.44 AM</t>
-  </si>
-  <si>
-    <t>tran6648717508</t>
-  </si>
-  <si>
-    <t>transaction16648717508</t>
-  </si>
-  <si>
-    <t>2218190426</t>
-  </si>
-  <si>
-    <t>3947572804</t>
-  </si>
-  <si>
-    <t>10.57 AM</t>
-  </si>
-  <si>
-    <t>tran3960952692</t>
-  </si>
-  <si>
-    <t>transaction13960952692</t>
-  </si>
-  <si>
-    <t>2888213631</t>
-  </si>
-  <si>
-    <t>3046133329</t>
-  </si>
-  <si>
-    <t>11.03 AM</t>
-  </si>
-  <si>
-    <t>tran7948168480</t>
-  </si>
-  <si>
-    <t>transaction17948168480</t>
-  </si>
-  <si>
-    <t>3520619702</t>
-  </si>
-  <si>
-    <t>7073974788</t>
-  </si>
-  <si>
-    <t>11.09 AM</t>
-  </si>
-  <si>
-    <t>tran6490486962</t>
-  </si>
-  <si>
-    <t>transaction16490486962</t>
-  </si>
-  <si>
-    <t>5399550501</t>
-  </si>
-  <si>
-    <t>1781489870</t>
-  </si>
-  <si>
-    <t>11.30 AM</t>
-  </si>
-  <si>
-    <t>tran9650383448</t>
-  </si>
-  <si>
-    <t>transaction19650383448</t>
-  </si>
-  <si>
-    <t>3780550546</t>
-  </si>
-  <si>
-    <t>6451863160</t>
-  </si>
-  <si>
-    <t>12.05 PM</t>
+    <t>01.15 PM</t>
   </si>
 </sst>
 </file>
@@ -2720,8 +2399,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CS3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="V1" sqref="V1"/>
+    <sheetView tabSelected="1" topLeftCell="BT1" workbookViewId="0">
+      <selection activeCell="BZ3" sqref="BZ3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -3112,10 +2791,10 @@
     </row>
     <row r="2" spans="1:97" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>764</v>
+        <v>657</v>
       </c>
       <c r="B2" t="s">
-        <v>766</v>
+        <v>659</v>
       </c>
       <c r="C2" t="s">
         <v>488</v>
@@ -3175,7 +2854,7 @@
         <v>109</v>
       </c>
       <c r="V2" t="s">
-        <v>768</v>
+        <v>661</v>
       </c>
       <c r="W2" s="1" t="s">
         <v>103</v>
@@ -3311,7 +2990,7 @@
         <v>97</v>
       </c>
       <c r="BZ2" t="s">
-        <v>97</v>
+        <v>655</v>
       </c>
       <c r="CA2" t="s">
         <v>97</v>
@@ -3373,10 +3052,10 @@
     </row>
     <row r="3" spans="1:97" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>765</v>
+        <v>658</v>
       </c>
       <c r="B3" t="s">
-        <v>767</v>
+        <v>660</v>
       </c>
       <c r="C3" t="s">
         <v>488</v>
@@ -3397,7 +3076,7 @@
         <v>109</v>
       </c>
       <c r="V3" t="s">
-        <v>768</v>
+        <v>661</v>
       </c>
       <c r="W3" s="1" t="s">
         <v>103</v>
@@ -3451,6 +3130,9 @@
       <c r="BU3" t="s">
         <v>632</v>
       </c>
+      <c r="BZ3" t="s">
+        <v>656</v>
+      </c>
       <c r="CP3" t="s">
         <v>643</v>
       </c>
@@ -3459,7 +3141,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:J1 F2:J2 L1:U1 L2:R2 T2 X2 AA2 AF2:AK2 BE2:BR2 BT2 BV2:CO2 CQ2:CS2 V2 W1:CS1" numberStoredAsText="1"/>
+    <ignoredError sqref="A1:J1 F2:J2 L1:U1 L2:R2 T2 X2 AA2 AF2:AK2 BE2:BR2 BT2 BV2:BY2 CQ2:CS2 V2 W1:CS1 CA2:CO2" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Change in failed test cases
</commit_message>
<xml_diff>
--- a/src/main/resources/Bulk_ConventionalTransactions_File.xlsx
+++ b/src/main/resources/Bulk_ConventionalTransactions_File.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24400" uniqueCount="662">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24430" uniqueCount="687">
   <si>
     <t>transactionName</t>
   </si>
@@ -2007,6 +2007,81 @@
   <si>
     <t>01.15 PM</t>
   </si>
+  <si>
+    <t>tran1701777874</t>
+  </si>
+  <si>
+    <t>transaction11701777874</t>
+  </si>
+  <si>
+    <t>8072939087</t>
+  </si>
+  <si>
+    <t>1146610959</t>
+  </si>
+  <si>
+    <t>04:35PM</t>
+  </si>
+  <si>
+    <t>tran7325848997</t>
+  </si>
+  <si>
+    <t>transaction17325848997</t>
+  </si>
+  <si>
+    <t>8767644689</t>
+  </si>
+  <si>
+    <t>8602283326</t>
+  </si>
+  <si>
+    <t>04:45PM</t>
+  </si>
+  <si>
+    <t>tran6719558367</t>
+  </si>
+  <si>
+    <t>transaction16719558367</t>
+  </si>
+  <si>
+    <t>6387599715</t>
+  </si>
+  <si>
+    <t>8708702105</t>
+  </si>
+  <si>
+    <t>07:01PM</t>
+  </si>
+  <si>
+    <t>tran2590826239</t>
+  </si>
+  <si>
+    <t>transaction12590826239</t>
+  </si>
+  <si>
+    <t>6464277473</t>
+  </si>
+  <si>
+    <t>1109635083</t>
+  </si>
+  <si>
+    <t>12:15PM</t>
+  </si>
+  <si>
+    <t>tran2005938160</t>
+  </si>
+  <si>
+    <t>transaction12005938160</t>
+  </si>
+  <si>
+    <t>2673510887</t>
+  </si>
+  <si>
+    <t>8117635140</t>
+  </si>
+  <si>
+    <t>04:17PM</t>
+  </si>
 </sst>
 </file>
 
@@ -2791,10 +2866,10 @@
     </row>
     <row r="2" spans="1:97" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>657</v>
+        <v>682</v>
       </c>
       <c r="B2" t="s">
-        <v>659</v>
+        <v>684</v>
       </c>
       <c r="C2" t="s">
         <v>488</v>
@@ -2854,7 +2929,7 @@
         <v>109</v>
       </c>
       <c r="V2" t="s">
-        <v>661</v>
+        <v>686</v>
       </c>
       <c r="W2" s="1" t="s">
         <v>103</v>
@@ -3052,10 +3127,10 @@
     </row>
     <row r="3" spans="1:97" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>658</v>
+        <v>683</v>
       </c>
       <c r="B3" t="s">
-        <v>660</v>
+        <v>685</v>
       </c>
       <c r="C3" t="s">
         <v>488</v>
@@ -3076,7 +3151,7 @@
         <v>109</v>
       </c>
       <c r="V3" t="s">
-        <v>661</v>
+        <v>686</v>
       </c>
       <c r="W3" s="1" t="s">
         <v>103</v>

</xml_diff>